<commit_message>
feat：update all star level and languge
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="1300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1316">
   <si>
     <t>int</t>
   </si>
@@ -3902,37 +3902,37 @@
     <t>RainbowText3</t>
   </si>
   <si>
-    <t>Level Count：{0}</t>
-  </si>
-  <si>
-    <t>关卡计数：{0}</t>
+    <t>Level Count：</t>
+  </si>
+  <si>
+    <t>关卡计数：</t>
   </si>
   <si>
     <t>RainbowText4</t>
   </si>
   <si>
-    <t>Star Count：{0}</t>
-  </si>
-  <si>
-    <t>获得星星：{0}</t>
+    <t>Star Count：</t>
+  </si>
+  <si>
+    <t>获得星星：</t>
   </si>
   <si>
     <t>RainbowText5</t>
   </si>
   <si>
-    <t>Time：{0}</t>
-  </si>
-  <si>
-    <t>时间：{0}</t>
+    <t>Time：</t>
+  </si>
+  <si>
+    <t>时间：</t>
   </si>
   <si>
     <t>RainbowText6</t>
   </si>
   <si>
-    <t>Total Star   {0}</t>
-  </si>
-  <si>
-    <t>星星总数   {0}</t>
+    <t xml:space="preserve">Total Star   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">星星总数   </t>
   </si>
   <si>
     <t>RainbowText7</t>
@@ -3942,6 +3942,54 @@
   </si>
   <si>
     <t>返回</t>
+  </si>
+  <si>
+    <t>RainbowText8</t>
+  </si>
+  <si>
+    <t>Pass a level</t>
+  </si>
+  <si>
+    <t>跳过一关</t>
+  </si>
+  <si>
+    <t>RainbowText9</t>
+  </si>
+  <si>
+    <t>RainbowText10</t>
+  </si>
+  <si>
+    <t>Your game count is insufficient！</t>
+  </si>
+  <si>
+    <t>你的游戏次数不足！</t>
+  </si>
+  <si>
+    <t>RainbowText11</t>
+  </si>
+  <si>
+    <t>Do you want to spend a game count to enter the Rainbow Run？</t>
+  </si>
+  <si>
+    <t>是否消耗一点游戏次数，进入rainbow跑酷？</t>
+  </si>
+  <si>
+    <t>RainbowText12</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>RainbowText13</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>否</t>
   </si>
 </sst>
 </file>
@@ -5014,8 +5062,8 @@
   <sheetPr/>
   <dimension ref="A1:H661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="C345" sqref="C345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -11617,12 +11665,90 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="339" s="2" customFormat="1"/>
-    <row r="340" s="2" customFormat="1"/>
-    <row r="341" s="2" customFormat="1"/>
-    <row r="342" s="2" customFormat="1"/>
-    <row r="343" s="2" customFormat="1"/>
-    <row r="344" s="2" customFormat="1"/>
+    <row r="339" s="2" customFormat="1" spans="1:4">
+      <c r="A339" s="2">
+        <v>300013</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C339" s="2" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D339" s="2" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="340" s="2" customFormat="1" spans="1:4">
+      <c r="A340" s="2">
+        <v>300014</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C340" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D340" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="341" s="2" customFormat="1" spans="1:4">
+      <c r="A341" s="2">
+        <v>300015</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C341" s="2" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D341" s="2" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="342" s="2" customFormat="1" spans="1:4">
+      <c r="A342" s="2">
+        <v>300016</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="343" s="2" customFormat="1" spans="1:4">
+      <c r="A343" s="2">
+        <v>300017</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D343" s="2" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="344" s="2" customFormat="1" spans="1:4">
+      <c r="A344" s="2">
+        <v>300018</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D344" s="2" t="s">
+        <v>1315</v>
+      </c>
+    </row>
     <row r="345" s="2" customFormat="1"/>
     <row r="346" s="2" customFormat="1"/>
     <row r="347" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat：update language and level change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="1316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="1331">
   <si>
     <t>int</t>
   </si>
@@ -3991,6 +3991,51 @@
   <si>
     <t>否</t>
   </si>
+  <si>
+    <t>addInvincible_Success</t>
+  </si>
+  <si>
+    <t>Enabling shield successfully！</t>
+  </si>
+  <si>
+    <t>添加护盾成功！</t>
+  </si>
+  <si>
+    <t>addInvincible_Fail</t>
+  </si>
+  <si>
+    <t>Enabling shield failed！</t>
+  </si>
+  <si>
+    <t>添加护盾失败！</t>
+  </si>
+  <si>
+    <t>Invincible_End</t>
+  </si>
+  <si>
+    <t>Shield end！</t>
+  </si>
+  <si>
+    <t>护盾结束！</t>
+  </si>
+  <si>
+    <t>autoFindPath_Fail</t>
+  </si>
+  <si>
+    <t>Automatic pathfinding failed！</t>
+  </si>
+  <si>
+    <t>自动寻路失败！</t>
+  </si>
+  <si>
+    <t>ObbyEnterWithoutTicket</t>
+  </si>
+  <si>
+    <t>Due to not failing in the last game，you do not counsume any game attempts this time！</t>
+  </si>
+  <si>
+    <t>由于上次在跑酷关内未失败，此次进入不消耗游戏次数！</t>
+  </si>
 </sst>
 </file>
 
@@ -4002,7 +4047,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4024,6 +4069,12 @@
       <sz val="12"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="微软雅黑"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4486,31 +4537,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4519,119 +4567,122 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4672,6 +4723,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5062,8 +5116,8 @@
   <sheetPr/>
   <dimension ref="A1:H661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="C345" sqref="C345"/>
+    <sheetView tabSelected="1" topLeftCell="A326" workbookViewId="0">
+      <selection activeCell="D350" sqref="D350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -11749,11 +11803,76 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="345" s="2" customFormat="1"/>
-    <row r="346" s="2" customFormat="1"/>
-    <row r="347" s="2" customFormat="1"/>
-    <row r="348" s="2" customFormat="1"/>
-    <row r="349" s="2" customFormat="1"/>
+    <row r="345" s="2" customFormat="1" spans="1:4">
+      <c r="A345" s="2">
+        <v>300019</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D345" s="2" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="346" s="2" customFormat="1" spans="1:4">
+      <c r="A346" s="2">
+        <v>300020</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D346" s="2" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="347" s="2" customFormat="1" spans="1:4">
+      <c r="A347" s="2">
+        <v>300021</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D347" s="2" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="348" s="2" customFormat="1" ht="17.25" spans="1:4">
+      <c r="A348" s="2">
+        <v>300022</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D348" s="15" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="349" s="2" customFormat="1" spans="1:4">
+      <c r="A349" s="2">
+        <v>300023</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D349" s="2" t="s">
+        <v>1330</v>
+      </c>
+    </row>
     <row r="350" s="2" customFormat="1"/>
     <row r="351" s="2" customFormat="1"/>
     <row r="352" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat: update Main_UI JumpHome_UI
更新主界面UI，增加跳转家园UI
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\dragon-verse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C10A716-9841-4BDE-A02F-322248CB9B66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DDFE33-BE2B-4B06-8CB0-6E0DE55BFC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4575,8 +4575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="F221" sqref="F221"/>
+    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="E349" sqref="E349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
feat:update map panel UI change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1715" uniqueCount="1356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1366">
   <si>
     <t>int</t>
   </si>
@@ -4110,6 +4110,36 @@
   </si>
   <si>
     <t>由于上次在跑酷关内未失败，此次进入不消耗游戏次数！</t>
+  </si>
+  <si>
+    <t>Maptext001</t>
+  </si>
+  <si>
+    <t>城堡跑酷</t>
+  </si>
+  <si>
+    <t>Maptext002</t>
+  </si>
+  <si>
+    <t>云端迷宫</t>
+  </si>
+  <si>
+    <t>Maptext003</t>
+  </si>
+  <si>
+    <t>火炎地狱</t>
+  </si>
+  <si>
+    <t>Maptext004</t>
+  </si>
+  <si>
+    <t>奶牛关</t>
+  </si>
+  <si>
+    <t>Maptext005</t>
+  </si>
+  <si>
+    <t>冰层</t>
   </si>
 </sst>
 </file>
@@ -4146,14 +4176,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="10.5"/>
+      <color rgb="FFCCCCCC"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FFCCCCCC"/>
+      <sz val="10"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -4789,12 +4818,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4811,8 +4834,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -5203,8 +5232,8 @@
   <sheetPr/>
   <dimension ref="A1:H676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B175" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+    <sheetView tabSelected="1" topLeftCell="D336" workbookViewId="0">
+      <selection activeCell="E359" sqref="E359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -9256,19 +9285,19 @@
       <c r="A211" s="1">
         <v>105701</v>
       </c>
-      <c r="B211" s="9" t="s">
+      <c r="B211" s="4" t="s">
         <v>818</v>
       </c>
-      <c r="C211" s="10" t="s">
+      <c r="C211" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D211" s="10" t="s">
+      <c r="D211" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="E211" s="10" t="s">
+      <c r="E211" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F211" s="10" t="s">
+      <c r="F211" s="3" t="s">
         <v>225</v>
       </c>
     </row>
@@ -9276,19 +9305,19 @@
       <c r="A212" s="1">
         <v>105702</v>
       </c>
-      <c r="B212" s="9" t="s">
+      <c r="B212" s="4" t="s">
         <v>820</v>
       </c>
-      <c r="C212" s="10" t="s">
+      <c r="C212" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="D212" s="10" t="s">
+      <c r="D212" s="3" t="s">
         <v>822</v>
       </c>
-      <c r="E212" s="10" t="s">
+      <c r="E212" s="3" t="s">
         <v>821</v>
       </c>
-      <c r="F212" s="10" t="s">
+      <c r="F212" s="3" t="s">
         <v>821</v>
       </c>
     </row>
@@ -9296,19 +9325,19 @@
       <c r="A213" s="1">
         <v>105703</v>
       </c>
-      <c r="B213" s="9" t="s">
+      <c r="B213" s="4" t="s">
         <v>823</v>
       </c>
-      <c r="C213" s="10" t="s">
+      <c r="C213" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="D213" s="10" t="s">
+      <c r="D213" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="E213" s="10" t="s">
+      <c r="E213" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="F213" s="10" t="s">
+      <c r="F213" s="3" t="s">
         <v>824</v>
       </c>
     </row>
@@ -9316,47 +9345,47 @@
       <c r="A214" s="1">
         <v>105704</v>
       </c>
-      <c r="B214" s="9" t="s">
+      <c r="B214" s="4" t="s">
         <v>826</v>
       </c>
-      <c r="C214" s="10" t="s">
+      <c r="C214" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="D214" s="10" t="s">
+      <c r="D214" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="E214" s="10" t="s">
+      <c r="E214" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="F214" s="10" t="s">
+      <c r="F214" s="3" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="215" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
       <c r="A215" s="1"/>
-      <c r="B215" s="9"/>
-      <c r="C215" s="10"/>
-      <c r="D215" s="10"/>
-      <c r="E215" s="10"/>
-      <c r="F215" s="10"/>
+      <c r="B215" s="4"/>
+      <c r="C215" s="3"/>
+      <c r="D215" s="3"/>
+      <c r="E215" s="3"/>
+      <c r="F215" s="3"/>
     </row>
     <row r="216" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
       <c r="A216" s="1">
         <v>105801</v>
       </c>
-      <c r="B216" s="9" t="s">
+      <c r="B216" s="4" t="s">
         <v>829</v>
       </c>
-      <c r="C216" s="10" t="s">
+      <c r="C216" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="D216" s="10" t="s">
+      <c r="D216" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="E216" s="10" t="s">
+      <c r="E216" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F216" s="10" t="s">
+      <c r="F216" s="3" t="s">
         <v>830</v>
       </c>
     </row>
@@ -9364,19 +9393,19 @@
       <c r="A217" s="1">
         <v>105802</v>
       </c>
-      <c r="B217" s="9" t="s">
+      <c r="B217" s="4" t="s">
         <v>832</v>
       </c>
-      <c r="C217" s="10" t="s">
+      <c r="C217" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="D217" s="10" t="s">
+      <c r="D217" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="E217" s="10" t="s">
+      <c r="E217" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F217" s="10" t="s">
+      <c r="F217" s="3" t="s">
         <v>830</v>
       </c>
     </row>
@@ -9384,19 +9413,19 @@
       <c r="A218" s="1">
         <v>105803</v>
       </c>
-      <c r="B218" s="9" t="s">
+      <c r="B218" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="C218" s="10" t="s">
+      <c r="C218" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="D218" s="10" t="s">
+      <c r="D218" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="E218" s="10" t="s">
+      <c r="E218" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F218" s="10" t="s">
+      <c r="F218" s="3" t="s">
         <v>830</v>
       </c>
     </row>
@@ -9404,1440 +9433,1440 @@
       <c r="A219" s="1">
         <v>105804</v>
       </c>
-      <c r="B219" s="9" t="s">
+      <c r="B219" s="4" t="s">
         <v>834</v>
       </c>
-      <c r="C219" s="10" t="s">
+      <c r="C219" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="D219" s="10" t="s">
+      <c r="D219" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="E219" s="10" t="s">
+      <c r="E219" s="3" t="s">
         <v>830</v>
       </c>
-      <c r="F219" s="10" t="s">
+      <c r="F219" s="3" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="220" s="2" customFormat="1" ht="18.75" customHeight="1"/>
     <row r="221" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A221" s="11">
+      <c r="A221" s="9">
         <v>200001</v>
       </c>
-      <c r="B221" s="11" t="s">
+      <c r="B221" s="9" t="s">
         <v>835</v>
       </c>
-      <c r="C221" s="12" t="s">
+      <c r="C221" s="10" t="s">
         <v>836</v>
       </c>
-      <c r="D221" s="12" t="s">
+      <c r="D221" s="10" t="s">
         <v>837</v>
       </c>
-      <c r="E221" s="13" t="s">
+      <c r="E221" s="11" t="s">
         <v>838</v>
       </c>
-      <c r="F221" s="13" t="s">
+      <c r="F221" s="11" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="222" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A222" s="11">
+      <c r="A222" s="9">
         <v>200002</v>
       </c>
-      <c r="B222" s="11" t="s">
+      <c r="B222" s="9" t="s">
         <v>839</v>
       </c>
-      <c r="C222" s="12" t="s">
+      <c r="C222" s="10" t="s">
         <v>840</v>
       </c>
-      <c r="D222" s="12" t="s">
+      <c r="D222" s="10" t="s">
         <v>841</v>
       </c>
-      <c r="E222" s="13" t="s">
+      <c r="E222" s="11" t="s">
         <v>842</v>
       </c>
-      <c r="F222" s="13" t="s">
+      <c r="F222" s="11" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="223" s="2" customFormat="1" spans="1:6">
-      <c r="A223" s="11">
+      <c r="A223" s="9">
         <v>200003</v>
       </c>
-      <c r="B223" s="11" t="s">
+      <c r="B223" s="9" t="s">
         <v>843</v>
       </c>
-      <c r="C223" s="12" t="s">
+      <c r="C223" s="10" t="s">
         <v>844</v>
       </c>
-      <c r="D223" s="12" t="s">
+      <c r="D223" s="10" t="s">
         <v>845</v>
       </c>
-      <c r="E223" s="13" t="s">
+      <c r="E223" s="11" t="s">
         <v>846</v>
       </c>
-      <c r="F223" s="13" t="s">
+      <c r="F223" s="11" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="224" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A224" s="11">
+      <c r="A224" s="9">
         <v>200004</v>
       </c>
-      <c r="B224" s="11" t="s">
+      <c r="B224" s="9" t="s">
         <v>847</v>
       </c>
-      <c r="C224" s="12" t="s">
+      <c r="C224" s="10" t="s">
         <v>848</v>
       </c>
-      <c r="D224" s="12" t="s">
+      <c r="D224" s="10" t="s">
         <v>849</v>
       </c>
-      <c r="E224" s="13" t="s">
+      <c r="E224" s="11" t="s">
         <v>850</v>
       </c>
-      <c r="F224" s="13" t="s">
+      <c r="F224" s="11" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="225" s="2" customFormat="1" spans="1:6">
-      <c r="A225" s="11">
+      <c r="A225" s="9">
         <v>200005</v>
       </c>
-      <c r="B225" s="11" t="s">
+      <c r="B225" s="9" t="s">
         <v>851</v>
       </c>
-      <c r="C225" s="12" t="s">
+      <c r="C225" s="10" t="s">
         <v>852</v>
       </c>
-      <c r="D225" s="12" t="s">
+      <c r="D225" s="10" t="s">
         <v>853</v>
       </c>
-      <c r="E225" s="13" t="s">
+      <c r="E225" s="11" t="s">
         <v>854</v>
       </c>
-      <c r="F225" s="13" t="s">
+      <c r="F225" s="11" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="226" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A226" s="11">
+      <c r="A226" s="9">
         <v>200006</v>
       </c>
-      <c r="B226" s="11" t="s">
+      <c r="B226" s="9" t="s">
         <v>855</v>
       </c>
-      <c r="C226" s="12" t="s">
+      <c r="C226" s="10" t="s">
         <v>856</v>
       </c>
-      <c r="D226" s="12" t="s">
+      <c r="D226" s="10" t="s">
         <v>857</v>
       </c>
-      <c r="E226" s="13" t="s">
+      <c r="E226" s="11" t="s">
         <v>858</v>
       </c>
-      <c r="F226" s="13" t="s">
+      <c r="F226" s="11" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="227" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A227" s="11">
+      <c r="A227" s="9">
         <v>200007</v>
       </c>
-      <c r="B227" s="11" t="s">
+      <c r="B227" s="9" t="s">
         <v>859</v>
       </c>
-      <c r="C227" s="12" t="s">
+      <c r="C227" s="10" t="s">
         <v>860</v>
       </c>
-      <c r="D227" s="12" t="s">
+      <c r="D227" s="10" t="s">
         <v>861</v>
       </c>
-      <c r="E227" s="13" t="s">
+      <c r="E227" s="11" t="s">
         <v>862</v>
       </c>
-      <c r="F227" s="13" t="s">
+      <c r="F227" s="11" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="228" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A228" s="11">
+      <c r="A228" s="9">
         <v>200008</v>
       </c>
-      <c r="B228" s="11" t="s">
+      <c r="B228" s="9" t="s">
         <v>863</v>
       </c>
-      <c r="C228" s="12" t="s">
+      <c r="C228" s="10" t="s">
         <v>864</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D228" s="10" t="s">
         <v>865</v>
       </c>
-      <c r="E228" s="13" t="s">
+      <c r="E228" s="11" t="s">
         <v>866</v>
       </c>
-      <c r="F228" s="13" t="s">
+      <c r="F228" s="11" t="s">
         <v>864</v>
       </c>
     </row>
     <row r="229" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A229" s="11">
+      <c r="A229" s="9">
         <v>200009</v>
       </c>
-      <c r="B229" s="11" t="s">
+      <c r="B229" s="9" t="s">
         <v>867</v>
       </c>
-      <c r="C229" s="12" t="s">
+      <c r="C229" s="10" t="s">
         <v>868</v>
       </c>
-      <c r="D229" s="12" t="s">
+      <c r="D229" s="10" t="s">
         <v>869</v>
       </c>
-      <c r="E229" s="13" t="s">
+      <c r="E229" s="11" t="s">
         <v>870</v>
       </c>
-      <c r="F229" s="13" t="s">
+      <c r="F229" s="11" t="s">
         <v>868</v>
       </c>
     </row>
     <row r="230" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A230" s="11">
+      <c r="A230" s="9">
         <v>200010</v>
       </c>
-      <c r="B230" s="11" t="s">
+      <c r="B230" s="9" t="s">
         <v>871</v>
       </c>
-      <c r="C230" s="12" t="s">
+      <c r="C230" s="10" t="s">
         <v>872</v>
       </c>
-      <c r="D230" s="12" t="s">
+      <c r="D230" s="10" t="s">
         <v>873</v>
       </c>
-      <c r="E230" s="13" t="s">
+      <c r="E230" s="11" t="s">
         <v>874</v>
       </c>
-      <c r="F230" s="13" t="s">
+      <c r="F230" s="11" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="231" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A231" s="11">
+      <c r="A231" s="9">
         <v>200011</v>
       </c>
-      <c r="B231" s="11" t="s">
+      <c r="B231" s="9" t="s">
         <v>875</v>
       </c>
-      <c r="C231" s="12" t="s">
+      <c r="C231" s="10" t="s">
         <v>876</v>
       </c>
-      <c r="D231" s="12" t="s">
+      <c r="D231" s="10" t="s">
         <v>877</v>
       </c>
-      <c r="E231" s="13" t="s">
+      <c r="E231" s="11" t="s">
         <v>878</v>
       </c>
-      <c r="F231" s="13" t="s">
+      <c r="F231" s="11" t="s">
         <v>876</v>
       </c>
     </row>
     <row r="232" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A232" s="11">
+      <c r="A232" s="9">
         <v>200012</v>
       </c>
-      <c r="B232" s="11" t="s">
+      <c r="B232" s="9" t="s">
         <v>879</v>
       </c>
-      <c r="C232" s="12" t="s">
+      <c r="C232" s="10" t="s">
         <v>880</v>
       </c>
-      <c r="D232" s="12" t="s">
+      <c r="D232" s="10" t="s">
         <v>881</v>
       </c>
-      <c r="E232" s="13" t="s">
+      <c r="E232" s="11" t="s">
         <v>882</v>
       </c>
-      <c r="F232" s="13" t="s">
+      <c r="F232" s="11" t="s">
         <v>880</v>
       </c>
     </row>
     <row r="233" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A233" s="11">
+      <c r="A233" s="9">
         <v>200013</v>
       </c>
-      <c r="B233" s="11" t="s">
+      <c r="B233" s="9" t="s">
         <v>883</v>
       </c>
-      <c r="C233" s="12" t="s">
+      <c r="C233" s="10" t="s">
         <v>884</v>
       </c>
-      <c r="D233" s="12" t="s">
+      <c r="D233" s="10" t="s">
         <v>885</v>
       </c>
-      <c r="E233" s="13" t="s">
+      <c r="E233" s="11" t="s">
         <v>886</v>
       </c>
-      <c r="F233" s="13" t="s">
+      <c r="F233" s="11" t="s">
         <v>884</v>
       </c>
     </row>
     <row r="234" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A234" s="11">
+      <c r="A234" s="9">
         <v>200014</v>
       </c>
-      <c r="B234" s="11" t="s">
+      <c r="B234" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="C234" s="12" t="s">
+      <c r="C234" s="10" t="s">
         <v>888</v>
       </c>
-      <c r="D234" s="12" t="s">
+      <c r="D234" s="10" t="s">
         <v>889</v>
       </c>
-      <c r="E234" s="13" t="s">
+      <c r="E234" s="11" t="s">
         <v>890</v>
       </c>
-      <c r="F234" s="13" t="s">
+      <c r="F234" s="11" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="235" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A235" s="11">
+      <c r="A235" s="9">
         <v>200015</v>
       </c>
-      <c r="B235" s="11" t="s">
+      <c r="B235" s="9" t="s">
         <v>891</v>
       </c>
-      <c r="C235" s="12" t="s">
+      <c r="C235" s="10" t="s">
         <v>892</v>
       </c>
-      <c r="D235" s="12" t="s">
+      <c r="D235" s="10" t="s">
         <v>893</v>
       </c>
-      <c r="E235" s="13" t="s">
+      <c r="E235" s="11" t="s">
         <v>894</v>
       </c>
-      <c r="F235" s="13" t="s">
+      <c r="F235" s="11" t="s">
         <v>892</v>
       </c>
     </row>
     <row r="236" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A236" s="11">
+      <c r="A236" s="9">
         <v>200016</v>
       </c>
-      <c r="B236" s="11" t="s">
+      <c r="B236" s="9" t="s">
         <v>895</v>
       </c>
-      <c r="C236" s="12" t="s">
+      <c r="C236" s="10" t="s">
         <v>896</v>
       </c>
-      <c r="D236" s="12" t="s">
+      <c r="D236" s="10" t="s">
         <v>897</v>
       </c>
-      <c r="E236" s="13" t="s">
+      <c r="E236" s="11" t="s">
         <v>898</v>
       </c>
-      <c r="F236" s="13" t="s">
+      <c r="F236" s="11" t="s">
         <v>896</v>
       </c>
     </row>
     <row r="237" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A237" s="11">
+      <c r="A237" s="9">
         <v>200017</v>
       </c>
-      <c r="B237" s="11" t="s">
+      <c r="B237" s="9" t="s">
         <v>899</v>
       </c>
-      <c r="C237" s="12" t="s">
+      <c r="C237" s="10" t="s">
         <v>900</v>
       </c>
-      <c r="D237" s="12" t="s">
+      <c r="D237" s="10" t="s">
         <v>901</v>
       </c>
-      <c r="E237" s="13" t="s">
+      <c r="E237" s="11" t="s">
         <v>902</v>
       </c>
-      <c r="F237" s="13" t="s">
+      <c r="F237" s="11" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="238" s="2" customFormat="1" spans="1:6">
-      <c r="A238" s="11">
+      <c r="A238" s="9">
         <v>200018</v>
       </c>
-      <c r="B238" s="11" t="s">
+      <c r="B238" s="9" t="s">
         <v>903</v>
       </c>
-      <c r="C238" s="12" t="s">
+      <c r="C238" s="10" t="s">
         <v>904</v>
       </c>
-      <c r="D238" s="12" t="s">
+      <c r="D238" s="10" t="s">
         <v>905</v>
       </c>
-      <c r="E238" s="13" t="s">
+      <c r="E238" s="11" t="s">
         <v>906</v>
       </c>
-      <c r="F238" s="13" t="s">
+      <c r="F238" s="11" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="239" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A239" s="11">
+      <c r="A239" s="9">
         <v>200019</v>
       </c>
-      <c r="B239" s="11" t="s">
+      <c r="B239" s="9" t="s">
         <v>907</v>
       </c>
-      <c r="C239" s="12" t="s">
+      <c r="C239" s="10" t="s">
         <v>908</v>
       </c>
-      <c r="D239" s="12" t="s">
+      <c r="D239" s="10" t="s">
         <v>909</v>
       </c>
-      <c r="E239" s="13" t="s">
+      <c r="E239" s="11" t="s">
         <v>910</v>
       </c>
-      <c r="F239" s="13" t="s">
+      <c r="F239" s="11" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="240" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A240" s="11">
+      <c r="A240" s="9">
         <v>200020</v>
       </c>
-      <c r="B240" s="11" t="s">
+      <c r="B240" s="9" t="s">
         <v>911</v>
       </c>
-      <c r="C240" s="12" t="s">
+      <c r="C240" s="10" t="s">
         <v>912</v>
       </c>
-      <c r="D240" s="12" t="s">
+      <c r="D240" s="10" t="s">
         <v>913</v>
       </c>
-      <c r="E240" s="13" t="s">
+      <c r="E240" s="11" t="s">
         <v>914</v>
       </c>
-      <c r="F240" s="13" t="s">
+      <c r="F240" s="11" t="s">
         <v>912</v>
       </c>
     </row>
     <row r="241" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A241" s="11">
+      <c r="A241" s="9">
         <v>200021</v>
       </c>
-      <c r="B241" s="11" t="s">
+      <c r="B241" s="9" t="s">
         <v>915</v>
       </c>
-      <c r="C241" s="12" t="s">
+      <c r="C241" s="10" t="s">
         <v>916</v>
       </c>
-      <c r="D241" s="12" t="s">
+      <c r="D241" s="10" t="s">
         <v>917</v>
       </c>
-      <c r="E241" s="13" t="s">
+      <c r="E241" s="11" t="s">
         <v>917</v>
       </c>
-      <c r="F241" s="13" t="s">
+      <c r="F241" s="11" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="242" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A242" s="11">
+      <c r="A242" s="9">
         <v>200022</v>
       </c>
-      <c r="B242" s="11" t="s">
+      <c r="B242" s="9" t="s">
         <v>918</v>
       </c>
-      <c r="C242" s="12" t="s">
+      <c r="C242" s="10" t="s">
         <v>919</v>
       </c>
-      <c r="D242" s="12" t="s">
+      <c r="D242" s="10" t="s">
         <v>920</v>
       </c>
-      <c r="E242" s="13" t="s">
+      <c r="E242" s="11" t="s">
         <v>921</v>
       </c>
-      <c r="F242" s="13" t="s">
+      <c r="F242" s="11" t="s">
         <v>919</v>
       </c>
     </row>
     <row r="243" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A243" s="11">
+      <c r="A243" s="9">
         <v>200023</v>
       </c>
-      <c r="B243" s="11" t="s">
+      <c r="B243" s="9" t="s">
         <v>922</v>
       </c>
-      <c r="C243" s="12" t="s">
+      <c r="C243" s="10" t="s">
         <v>923</v>
       </c>
-      <c r="D243" s="12" t="s">
+      <c r="D243" s="10" t="s">
         <v>924</v>
       </c>
-      <c r="E243" s="13" t="s">
+      <c r="E243" s="11" t="s">
         <v>925</v>
       </c>
-      <c r="F243" s="13" t="s">
+      <c r="F243" s="11" t="s">
         <v>923</v>
       </c>
     </row>
     <row r="244" s="2" customFormat="1" spans="1:6">
-      <c r="A244" s="11">
+      <c r="A244" s="9">
         <v>200024</v>
       </c>
-      <c r="B244" s="11" t="s">
+      <c r="B244" s="9" t="s">
         <v>926</v>
       </c>
-      <c r="C244" s="12" t="s">
+      <c r="C244" s="10" t="s">
         <v>927</v>
       </c>
-      <c r="D244" s="12" t="s">
+      <c r="D244" s="10" t="s">
         <v>928</v>
       </c>
-      <c r="E244" s="13" t="s">
+      <c r="E244" s="11" t="s">
         <v>929</v>
       </c>
-      <c r="F244" s="13" t="s">
+      <c r="F244" s="11" t="s">
         <v>927</v>
       </c>
     </row>
     <row r="245" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A245" s="11">
+      <c r="A245" s="9">
         <v>200025</v>
       </c>
-      <c r="B245" s="11" t="s">
+      <c r="B245" s="9" t="s">
         <v>930</v>
       </c>
-      <c r="C245" s="12" t="s">
+      <c r="C245" s="10" t="s">
         <v>931</v>
       </c>
-      <c r="D245" s="12" t="s">
+      <c r="D245" s="10" t="s">
         <v>932</v>
       </c>
-      <c r="E245" s="13" t="s">
+      <c r="E245" s="11" t="s">
         <v>933</v>
       </c>
-      <c r="F245" s="13" t="s">
+      <c r="F245" s="11" t="s">
         <v>931</v>
       </c>
     </row>
     <row r="246" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A246" s="11">
+      <c r="A246" s="9">
         <v>200026</v>
       </c>
-      <c r="B246" s="11" t="s">
+      <c r="B246" s="9" t="s">
         <v>934</v>
       </c>
-      <c r="C246" s="12" t="s">
+      <c r="C246" s="10" t="s">
         <v>935</v>
       </c>
-      <c r="D246" s="12" t="s">
+      <c r="D246" s="10" t="s">
         <v>936</v>
       </c>
-      <c r="E246" s="13" t="s">
+      <c r="E246" s="11" t="s">
         <v>937</v>
       </c>
-      <c r="F246" s="13" t="s">
+      <c r="F246" s="11" t="s">
         <v>935</v>
       </c>
     </row>
     <row r="247" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A247" s="11">
+      <c r="A247" s="9">
         <v>200027</v>
       </c>
-      <c r="B247" s="11" t="s">
+      <c r="B247" s="9" t="s">
         <v>938</v>
       </c>
-      <c r="C247" s="12" t="s">
+      <c r="C247" s="10" t="s">
         <v>939</v>
       </c>
-      <c r="D247" s="12" t="s">
+      <c r="D247" s="10" t="s">
         <v>940</v>
       </c>
-      <c r="E247" s="13" t="s">
+      <c r="E247" s="11" t="s">
         <v>941</v>
       </c>
-      <c r="F247" s="13" t="s">
+      <c r="F247" s="11" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="248" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A248" s="11">
+      <c r="A248" s="9">
         <v>200028</v>
       </c>
-      <c r="B248" s="11" t="s">
+      <c r="B248" s="9" t="s">
         <v>942</v>
       </c>
-      <c r="C248" s="12" t="s">
+      <c r="C248" s="10" t="s">
         <v>943</v>
       </c>
-      <c r="D248" s="12" t="s">
+      <c r="D248" s="10" t="s">
         <v>944</v>
       </c>
-      <c r="E248" s="13" t="s">
+      <c r="E248" s="11" t="s">
         <v>945</v>
       </c>
-      <c r="F248" s="13" t="s">
+      <c r="F248" s="11" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="249" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A249" s="11">
+      <c r="A249" s="9">
         <v>200029</v>
       </c>
-      <c r="B249" s="11" t="s">
+      <c r="B249" s="9" t="s">
         <v>946</v>
       </c>
-      <c r="C249" s="12" t="s">
+      <c r="C249" s="10" t="s">
         <v>947</v>
       </c>
-      <c r="D249" s="12" t="s">
+      <c r="D249" s="10" t="s">
         <v>948</v>
       </c>
-      <c r="E249" s="13" t="s">
+      <c r="E249" s="11" t="s">
         <v>949</v>
       </c>
-      <c r="F249" s="13" t="s">
+      <c r="F249" s="11" t="s">
         <v>947</v>
       </c>
     </row>
     <row r="250" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A250" s="11">
+      <c r="A250" s="9">
         <v>200030</v>
       </c>
-      <c r="B250" s="11" t="s">
+      <c r="B250" s="9" t="s">
         <v>950</v>
       </c>
-      <c r="C250" s="12" t="s">
+      <c r="C250" s="10" t="s">
         <v>951</v>
       </c>
-      <c r="D250" s="12" t="s">
+      <c r="D250" s="10" t="s">
         <v>952</v>
       </c>
-      <c r="E250" s="13" t="s">
+      <c r="E250" s="11" t="s">
         <v>953</v>
       </c>
-      <c r="F250" s="13" t="s">
+      <c r="F250" s="11" t="s">
         <v>951</v>
       </c>
     </row>
     <row r="251" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A251" s="11">
+      <c r="A251" s="9">
         <v>200031</v>
       </c>
-      <c r="B251" s="11" t="s">
+      <c r="B251" s="9" t="s">
         <v>954</v>
       </c>
-      <c r="C251" s="12" t="s">
+      <c r="C251" s="10" t="s">
         <v>955</v>
       </c>
-      <c r="D251" s="12" t="s">
+      <c r="D251" s="10" t="s">
         <v>956</v>
       </c>
-      <c r="E251" s="13" t="s">
+      <c r="E251" s="11" t="s">
         <v>957</v>
       </c>
-      <c r="F251" s="13" t="s">
+      <c r="F251" s="11" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="252" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A252" s="11">
+      <c r="A252" s="9">
         <v>200032</v>
       </c>
-      <c r="B252" s="11" t="s">
+      <c r="B252" s="9" t="s">
         <v>958</v>
       </c>
-      <c r="C252" s="12" t="s">
+      <c r="C252" s="10" t="s">
         <v>959</v>
       </c>
-      <c r="D252" s="12" t="s">
+      <c r="D252" s="10" t="s">
         <v>960</v>
       </c>
-      <c r="E252" s="13" t="s">
+      <c r="E252" s="11" t="s">
         <v>961</v>
       </c>
-      <c r="F252" s="13" t="s">
+      <c r="F252" s="11" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="253" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A253" s="11">
+      <c r="A253" s="9">
         <v>200033</v>
       </c>
-      <c r="B253" s="11" t="s">
+      <c r="B253" s="9" t="s">
         <v>962</v>
       </c>
-      <c r="C253" s="12" t="s">
+      <c r="C253" s="10" t="s">
         <v>963</v>
       </c>
-      <c r="D253" s="12" t="s">
+      <c r="D253" s="10" t="s">
         <v>964</v>
       </c>
-      <c r="E253" s="13" t="s">
+      <c r="E253" s="11" t="s">
         <v>965</v>
       </c>
-      <c r="F253" s="13" t="s">
+      <c r="F253" s="11" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="254" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A254" s="11">
+      <c r="A254" s="9">
         <v>200034</v>
       </c>
-      <c r="B254" s="11" t="s">
+      <c r="B254" s="9" t="s">
         <v>966</v>
       </c>
-      <c r="C254" s="12" t="s">
+      <c r="C254" s="10" t="s">
         <v>967</v>
       </c>
-      <c r="D254" s="12" t="s">
+      <c r="D254" s="10" t="s">
         <v>968</v>
       </c>
-      <c r="E254" s="13" t="s">
+      <c r="E254" s="11" t="s">
         <v>969</v>
       </c>
-      <c r="F254" s="13" t="s">
+      <c r="F254" s="11" t="s">
         <v>967</v>
       </c>
     </row>
     <row r="255" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A255" s="11">
+      <c r="A255" s="9">
         <v>200035</v>
       </c>
-      <c r="B255" s="11" t="s">
+      <c r="B255" s="9" t="s">
         <v>970</v>
       </c>
-      <c r="C255" s="12" t="s">
+      <c r="C255" s="10" t="s">
         <v>971</v>
       </c>
-      <c r="D255" s="12" t="s">
+      <c r="D255" s="10" t="s">
         <v>972</v>
       </c>
-      <c r="E255" s="13" t="s">
+      <c r="E255" s="11" t="s">
         <v>973</v>
       </c>
-      <c r="F255" s="13" t="s">
+      <c r="F255" s="11" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="256" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A256" s="11">
+      <c r="A256" s="9">
         <v>200036</v>
       </c>
-      <c r="B256" s="11" t="s">
+      <c r="B256" s="9" t="s">
         <v>974</v>
       </c>
-      <c r="C256" s="12" t="s">
+      <c r="C256" s="10" t="s">
         <v>975</v>
       </c>
-      <c r="D256" s="12" t="s">
+      <c r="D256" s="10" t="s">
         <v>976</v>
       </c>
-      <c r="E256" s="13" t="s">
+      <c r="E256" s="11" t="s">
         <v>977</v>
       </c>
-      <c r="F256" s="13" t="s">
+      <c r="F256" s="11" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="257" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A257" s="11">
+      <c r="A257" s="9">
         <v>200037</v>
       </c>
-      <c r="B257" s="11" t="s">
+      <c r="B257" s="9" t="s">
         <v>978</v>
       </c>
-      <c r="C257" s="12" t="s">
+      <c r="C257" s="10" t="s">
         <v>979</v>
       </c>
-      <c r="D257" s="12" t="s">
+      <c r="D257" s="10" t="s">
         <v>980</v>
       </c>
-      <c r="E257" s="13" t="s">
+      <c r="E257" s="11" t="s">
         <v>981</v>
       </c>
-      <c r="F257" s="13" t="s">
+      <c r="F257" s="11" t="s">
         <v>979</v>
       </c>
     </row>
     <row r="258" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A258" s="11">
+      <c r="A258" s="9">
         <v>200038</v>
       </c>
-      <c r="B258" s="11" t="s">
+      <c r="B258" s="9" t="s">
         <v>982</v>
       </c>
-      <c r="C258" s="12" t="s">
+      <c r="C258" s="10" t="s">
         <v>983</v>
       </c>
-      <c r="D258" s="12" t="s">
+      <c r="D258" s="10" t="s">
         <v>984</v>
       </c>
-      <c r="E258" s="13" t="s">
+      <c r="E258" s="11" t="s">
         <v>985</v>
       </c>
-      <c r="F258" s="13" t="s">
+      <c r="F258" s="11" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="259" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A259" s="11">
+      <c r="A259" s="9">
         <v>200039</v>
       </c>
-      <c r="B259" s="11" t="s">
+      <c r="B259" s="9" t="s">
         <v>986</v>
       </c>
-      <c r="C259" s="12" t="s">
+      <c r="C259" s="10" t="s">
         <v>987</v>
       </c>
-      <c r="D259" s="12" t="s">
+      <c r="D259" s="10" t="s">
         <v>988</v>
       </c>
-      <c r="E259" s="13" t="s">
+      <c r="E259" s="11" t="s">
         <v>989</v>
       </c>
-      <c r="F259" s="13" t="s">
+      <c r="F259" s="11" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="260" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A260" s="11">
+      <c r="A260" s="9">
         <v>200040</v>
       </c>
-      <c r="B260" s="11" t="s">
+      <c r="B260" s="9" t="s">
         <v>990</v>
       </c>
-      <c r="C260" s="13" t="s">
+      <c r="C260" s="11" t="s">
         <v>991</v>
       </c>
-      <c r="D260" s="14" t="s">
+      <c r="D260" s="12" t="s">
         <v>992</v>
       </c>
-      <c r="E260" s="13" t="s">
+      <c r="E260" s="11" t="s">
         <v>993</v>
       </c>
-      <c r="F260" s="13" t="s">
+      <c r="F260" s="11" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="261" s="2" customFormat="1" spans="1:6">
-      <c r="A261" s="11">
+      <c r="A261" s="9">
         <v>200041</v>
       </c>
-      <c r="B261" s="11" t="s">
+      <c r="B261" s="9" t="s">
         <v>994</v>
       </c>
-      <c r="C261" s="14" t="s">
+      <c r="C261" s="12" t="s">
         <v>995</v>
       </c>
-      <c r="D261" s="14" t="s">
+      <c r="D261" s="12" t="s">
         <v>996</v>
       </c>
-      <c r="E261" s="13" t="s">
+      <c r="E261" s="11" t="s">
         <v>997</v>
       </c>
-      <c r="F261" s="13" t="s">
+      <c r="F261" s="11" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="262" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A262" s="11">
+      <c r="A262" s="9">
         <v>200042</v>
       </c>
-      <c r="B262" s="11" t="s">
+      <c r="B262" s="9" t="s">
         <v>998</v>
       </c>
-      <c r="C262" s="14" t="s">
+      <c r="C262" s="12" t="s">
         <v>999</v>
       </c>
-      <c r="D262" s="13" t="s">
+      <c r="D262" s="11" t="s">
         <v>1000</v>
       </c>
-      <c r="E262" s="13" t="s">
+      <c r="E262" s="11" t="s">
         <v>1001</v>
       </c>
-      <c r="F262" s="13" t="s">
+      <c r="F262" s="11" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="263" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A263" s="11">
+      <c r="A263" s="9">
         <v>200043</v>
       </c>
-      <c r="B263" s="11" t="s">
+      <c r="B263" s="9" t="s">
         <v>1002</v>
       </c>
-      <c r="C263" s="13" t="s">
+      <c r="C263" s="11" t="s">
         <v>1003</v>
       </c>
-      <c r="D263" s="13" t="s">
+      <c r="D263" s="11" t="s">
         <v>1004</v>
       </c>
-      <c r="E263" s="13" t="s">
+      <c r="E263" s="11" t="s">
         <v>1005</v>
       </c>
-      <c r="F263" s="13" t="s">
+      <c r="F263" s="11" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="264" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A264" s="11">
+      <c r="A264" s="9">
         <v>200044</v>
       </c>
-      <c r="B264" s="11" t="s">
+      <c r="B264" s="9" t="s">
         <v>1006</v>
       </c>
-      <c r="C264" s="13" t="s">
+      <c r="C264" s="11" t="s">
         <v>1007</v>
       </c>
-      <c r="D264" s="13" t="s">
+      <c r="D264" s="11" t="s">
         <v>1008</v>
       </c>
-      <c r="E264" s="13" t="s">
+      <c r="E264" s="11" t="s">
         <v>1009</v>
       </c>
-      <c r="F264" s="13" t="s">
+      <c r="F264" s="11" t="s">
         <v>1007</v>
       </c>
     </row>
     <row r="265" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A265" s="11">
+      <c r="A265" s="9">
         <v>200045</v>
       </c>
-      <c r="B265" s="11" t="s">
+      <c r="B265" s="9" t="s">
         <v>1010</v>
       </c>
-      <c r="C265" s="13" t="s">
+      <c r="C265" s="11" t="s">
         <v>1011</v>
       </c>
-      <c r="D265" s="13" t="s">
+      <c r="D265" s="11" t="s">
         <v>1012</v>
       </c>
-      <c r="E265" s="13" t="s">
+      <c r="E265" s="11" t="s">
         <v>1013</v>
       </c>
-      <c r="F265" s="13" t="s">
+      <c r="F265" s="11" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="266" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A266" s="11">
+      <c r="A266" s="9">
         <v>200046</v>
       </c>
-      <c r="B266" s="11" t="s">
+      <c r="B266" s="9" t="s">
         <v>1014</v>
       </c>
-      <c r="C266" s="13" t="s">
+      <c r="C266" s="11" t="s">
         <v>1015</v>
       </c>
-      <c r="D266" s="13" t="s">
+      <c r="D266" s="11" t="s">
         <v>1016</v>
       </c>
-      <c r="E266" s="13" t="s">
+      <c r="E266" s="11" t="s">
         <v>1017</v>
       </c>
-      <c r="F266" s="13" t="s">
+      <c r="F266" s="11" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="267" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A267" s="11">
+      <c r="A267" s="9">
         <v>200047</v>
       </c>
-      <c r="B267" s="11" t="s">
+      <c r="B267" s="9" t="s">
         <v>1018</v>
       </c>
-      <c r="C267" s="14" t="s">
+      <c r="C267" s="12" t="s">
         <v>1019</v>
       </c>
-      <c r="D267" s="14" t="s">
+      <c r="D267" s="12" t="s">
         <v>1020</v>
       </c>
-      <c r="E267" s="13" t="s">
+      <c r="E267" s="11" t="s">
         <v>1021</v>
       </c>
-      <c r="F267" s="13" t="s">
+      <c r="F267" s="11" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="268" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A268" s="11">
+      <c r="A268" s="9">
         <v>200048</v>
       </c>
-      <c r="B268" s="11" t="s">
+      <c r="B268" s="9" t="s">
         <v>1022</v>
       </c>
-      <c r="C268" s="13" t="s">
+      <c r="C268" s="11" t="s">
         <v>1023</v>
       </c>
-      <c r="D268" s="13" t="s">
+      <c r="D268" s="11" t="s">
         <v>1024</v>
       </c>
-      <c r="E268" s="13" t="s">
+      <c r="E268" s="11" t="s">
         <v>1025</v>
       </c>
-      <c r="F268" s="13" t="s">
+      <c r="F268" s="11" t="s">
         <v>1023</v>
       </c>
     </row>
     <row r="269" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A269" s="11">
+      <c r="A269" s="9">
         <v>200049</v>
       </c>
-      <c r="B269" s="11" t="s">
+      <c r="B269" s="9" t="s">
         <v>1026</v>
       </c>
-      <c r="C269" s="14" t="s">
+      <c r="C269" s="12" t="s">
         <v>1027</v>
       </c>
-      <c r="D269" s="14" t="s">
+      <c r="D269" s="12" t="s">
         <v>1028</v>
       </c>
-      <c r="E269" s="13" t="s">
+      <c r="E269" s="11" t="s">
         <v>1029</v>
       </c>
-      <c r="F269" s="13" t="s">
+      <c r="F269" s="11" t="s">
         <v>1027</v>
       </c>
     </row>
     <row r="270" s="2" customFormat="1" spans="1:6">
-      <c r="A270" s="11">
+      <c r="A270" s="9">
         <v>200050</v>
       </c>
-      <c r="B270" s="11" t="s">
+      <c r="B270" s="9" t="s">
         <v>1030</v>
       </c>
-      <c r="C270" s="14" t="s">
+      <c r="C270" s="12" t="s">
         <v>1031</v>
       </c>
-      <c r="D270" s="14" t="s">
+      <c r="D270" s="12" t="s">
         <v>1032</v>
       </c>
-      <c r="E270" s="13" t="s">
+      <c r="E270" s="11" t="s">
         <v>1033</v>
       </c>
-      <c r="F270" s="13" t="s">
+      <c r="F270" s="11" t="s">
         <v>1031</v>
       </c>
     </row>
     <row r="271" s="2" customFormat="1" spans="1:6">
-      <c r="A271" s="11">
+      <c r="A271" s="9">
         <v>200051</v>
       </c>
-      <c r="B271" s="11" t="s">
+      <c r="B271" s="9" t="s">
         <v>1034</v>
       </c>
-      <c r="C271" s="13" t="s">
+      <c r="C271" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="D271" s="13" t="s">
+      <c r="D271" s="11" t="s">
         <v>1036</v>
       </c>
-      <c r="E271" s="13" t="s">
+      <c r="E271" s="11" t="s">
         <v>1037</v>
       </c>
-      <c r="F271" s="13" t="s">
+      <c r="F271" s="11" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="272" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A272" s="11">
+      <c r="A272" s="9">
         <v>200052</v>
       </c>
-      <c r="B272" s="11" t="s">
+      <c r="B272" s="9" t="s">
         <v>1038</v>
       </c>
-      <c r="C272" s="13" t="s">
+      <c r="C272" s="11" t="s">
         <v>1039</v>
       </c>
-      <c r="D272" s="13" t="s">
+      <c r="D272" s="11" t="s">
         <v>1040</v>
       </c>
-      <c r="E272" s="13" t="s">
+      <c r="E272" s="11" t="s">
         <v>1041</v>
       </c>
-      <c r="F272" s="13" t="s">
+      <c r="F272" s="11" t="s">
         <v>1039</v>
       </c>
     </row>
     <row r="273" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A273" s="11">
+      <c r="A273" s="9">
         <v>200053</v>
       </c>
-      <c r="B273" s="11" t="s">
+      <c r="B273" s="9" t="s">
         <v>1042</v>
       </c>
-      <c r="C273" s="13" t="s">
+      <c r="C273" s="11" t="s">
         <v>1043</v>
       </c>
-      <c r="D273" s="13" t="s">
+      <c r="D273" s="11" t="s">
         <v>1044</v>
       </c>
-      <c r="E273" s="13" t="s">
+      <c r="E273" s="11" t="s">
         <v>1045</v>
       </c>
-      <c r="F273" s="13" t="s">
+      <c r="F273" s="11" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="274" s="2" customFormat="1" spans="1:6">
-      <c r="A274" s="11">
+      <c r="A274" s="9">
         <v>200054</v>
       </c>
-      <c r="B274" s="11" t="s">
+      <c r="B274" s="9" t="s">
         <v>1046</v>
       </c>
-      <c r="C274" s="13" t="s">
+      <c r="C274" s="11" t="s">
         <v>1047</v>
       </c>
-      <c r="D274" s="13" t="s">
+      <c r="D274" s="11" t="s">
         <v>1048</v>
       </c>
-      <c r="E274" s="13" t="s">
+      <c r="E274" s="11" t="s">
         <v>1049</v>
       </c>
-      <c r="F274" s="13" t="s">
+      <c r="F274" s="11" t="s">
         <v>1047</v>
       </c>
     </row>
     <row r="275" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A275" s="11">
+      <c r="A275" s="9">
         <v>200055</v>
       </c>
-      <c r="B275" s="11" t="s">
+      <c r="B275" s="9" t="s">
         <v>1050</v>
       </c>
-      <c r="C275" s="13" t="s">
+      <c r="C275" s="11" t="s">
         <v>1051</v>
       </c>
-      <c r="D275" s="13" t="s">
+      <c r="D275" s="11" t="s">
         <v>1052</v>
       </c>
-      <c r="E275" s="13" t="s">
+      <c r="E275" s="11" t="s">
         <v>1053</v>
       </c>
-      <c r="F275" s="13" t="s">
+      <c r="F275" s="11" t="s">
         <v>1051</v>
       </c>
     </row>
     <row r="276" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A276" s="11">
+      <c r="A276" s="9">
         <v>200056</v>
       </c>
-      <c r="B276" s="11" t="s">
+      <c r="B276" s="9" t="s">
         <v>1054</v>
       </c>
-      <c r="C276" s="14" t="s">
+      <c r="C276" s="12" t="s">
         <v>1055</v>
       </c>
-      <c r="D276" s="14" t="s">
+      <c r="D276" s="12" t="s">
         <v>1056</v>
       </c>
-      <c r="E276" s="13" t="s">
+      <c r="E276" s="11" t="s">
         <v>1057</v>
       </c>
-      <c r="F276" s="13" t="s">
+      <c r="F276" s="11" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="277" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A277" s="11">
+      <c r="A277" s="9">
         <v>200057</v>
       </c>
-      <c r="B277" s="11" t="s">
+      <c r="B277" s="9" t="s">
         <v>1058</v>
       </c>
-      <c r="C277" s="13" t="s">
+      <c r="C277" s="11" t="s">
         <v>1059</v>
       </c>
-      <c r="D277" s="13" t="s">
+      <c r="D277" s="11" t="s">
         <v>1060</v>
       </c>
-      <c r="E277" s="13" t="s">
+      <c r="E277" s="11" t="s">
         <v>1061</v>
       </c>
-      <c r="F277" s="13" t="s">
+      <c r="F277" s="11" t="s">
         <v>1059</v>
       </c>
     </row>
     <row r="278" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A278" s="11">
+      <c r="A278" s="9">
         <v>200058</v>
       </c>
-      <c r="B278" s="11" t="s">
+      <c r="B278" s="9" t="s">
         <v>1062</v>
       </c>
-      <c r="C278" s="14" t="s">
+      <c r="C278" s="12" t="s">
         <v>1063</v>
       </c>
-      <c r="D278" s="14" t="s">
+      <c r="D278" s="12" t="s">
         <v>1064</v>
       </c>
-      <c r="E278" s="13" t="s">
+      <c r="E278" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="F278" s="13" t="s">
+      <c r="F278" s="11" t="s">
         <v>1063</v>
       </c>
     </row>
     <row r="279" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A279" s="11">
+      <c r="A279" s="9">
         <v>200059</v>
       </c>
-      <c r="B279" s="11" t="s">
+      <c r="B279" s="9" t="s">
         <v>1066</v>
       </c>
-      <c r="C279" s="14" t="s">
+      <c r="C279" s="12" t="s">
         <v>1067</v>
       </c>
-      <c r="D279" s="14" t="s">
+      <c r="D279" s="12" t="s">
         <v>1068</v>
       </c>
-      <c r="E279" s="13" t="s">
+      <c r="E279" s="11" t="s">
         <v>1069</v>
       </c>
-      <c r="F279" s="13" t="s">
+      <c r="F279" s="11" t="s">
         <v>1067</v>
       </c>
     </row>
     <row r="280" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A280" s="11">
+      <c r="A280" s="9">
         <v>200060</v>
       </c>
-      <c r="B280" s="11" t="s">
+      <c r="B280" s="9" t="s">
         <v>1070</v>
       </c>
-      <c r="C280" s="13" t="s">
+      <c r="C280" s="11" t="s">
         <v>1071</v>
       </c>
-      <c r="D280" s="14" t="s">
+      <c r="D280" s="12" t="s">
         <v>1072</v>
       </c>
-      <c r="E280" s="13" t="s">
+      <c r="E280" s="11" t="s">
         <v>1073</v>
       </c>
-      <c r="F280" s="13" t="s">
+      <c r="F280" s="11" t="s">
         <v>1071</v>
       </c>
     </row>
     <row r="281" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A281" s="11">
+      <c r="A281" s="9">
         <v>200061</v>
       </c>
-      <c r="B281" s="11" t="s">
+      <c r="B281" s="9" t="s">
         <v>1074</v>
       </c>
-      <c r="C281" s="13" t="s">
+      <c r="C281" s="11" t="s">
         <v>1075</v>
       </c>
-      <c r="D281" s="13" t="s">
+      <c r="D281" s="11" t="s">
         <v>1076</v>
       </c>
-      <c r="E281" s="13" t="s">
+      <c r="E281" s="11" t="s">
         <v>1077</v>
       </c>
-      <c r="F281" s="13" t="s">
+      <c r="F281" s="11" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="282" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A282" s="11">
+      <c r="A282" s="9">
         <v>200062</v>
       </c>
-      <c r="B282" s="11" t="s">
+      <c r="B282" s="9" t="s">
         <v>1078</v>
       </c>
-      <c r="C282" s="13" t="s">
+      <c r="C282" s="11" t="s">
         <v>1079</v>
       </c>
-      <c r="D282" s="14" t="s">
+      <c r="D282" s="12" t="s">
         <v>1080</v>
       </c>
-      <c r="E282" s="13" t="s">
+      <c r="E282" s="11" t="s">
         <v>1081</v>
       </c>
-      <c r="F282" s="13" t="s">
+      <c r="F282" s="11" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="283" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A283" s="11">
+      <c r="A283" s="9">
         <v>200063</v>
       </c>
-      <c r="B283" s="11" t="s">
+      <c r="B283" s="9" t="s">
         <v>1082</v>
       </c>
-      <c r="C283" s="14" t="s">
+      <c r="C283" s="12" t="s">
         <v>1083</v>
       </c>
-      <c r="D283" s="14" t="s">
+      <c r="D283" s="12" t="s">
         <v>1056</v>
       </c>
-      <c r="E283" s="13" t="s">
+      <c r="E283" s="11" t="s">
         <v>1057</v>
       </c>
-      <c r="F283" s="13" t="s">
+      <c r="F283" s="11" t="s">
         <v>1083</v>
       </c>
     </row>
     <row r="284" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A284" s="11">
+      <c r="A284" s="9">
         <v>200064</v>
       </c>
-      <c r="B284" s="11" t="s">
+      <c r="B284" s="9" t="s">
         <v>1084</v>
       </c>
-      <c r="C284" s="14" t="s">
+      <c r="C284" s="12" t="s">
         <v>1085</v>
       </c>
-      <c r="D284" s="14" t="s">
+      <c r="D284" s="12" t="s">
         <v>1086</v>
       </c>
-      <c r="E284" s="13" t="s">
+      <c r="E284" s="11" t="s">
         <v>1087</v>
       </c>
-      <c r="F284" s="13" t="s">
+      <c r="F284" s="11" t="s">
         <v>1085</v>
       </c>
     </row>
     <row r="285" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A285" s="11">
+      <c r="A285" s="9">
         <v>200065</v>
       </c>
-      <c r="B285" s="11" t="s">
+      <c r="B285" s="9" t="s">
         <v>1088</v>
       </c>
-      <c r="C285" s="14" t="s">
+      <c r="C285" s="12" t="s">
         <v>1089</v>
       </c>
-      <c r="D285" s="14" t="s">
+      <c r="D285" s="12" t="s">
         <v>1090</v>
       </c>
-      <c r="E285" s="13" t="s">
+      <c r="E285" s="11" t="s">
         <v>1091</v>
       </c>
-      <c r="F285" s="13" t="s">
+      <c r="F285" s="11" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="286" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A286" s="11">
+      <c r="A286" s="9">
         <v>200066</v>
       </c>
-      <c r="B286" s="11" t="s">
+      <c r="B286" s="9" t="s">
         <v>1092</v>
       </c>
-      <c r="C286" s="14" t="s">
+      <c r="C286" s="12" t="s">
         <v>1093</v>
       </c>
-      <c r="D286" s="14" t="s">
+      <c r="D286" s="12" t="s">
         <v>1094</v>
       </c>
-      <c r="E286" s="13" t="s">
+      <c r="E286" s="11" t="s">
         <v>1095</v>
       </c>
-      <c r="F286" s="13" t="s">
+      <c r="F286" s="11" t="s">
         <v>1093</v>
       </c>
     </row>
     <row r="287" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A287" s="11">
+      <c r="A287" s="9">
         <v>200067</v>
       </c>
-      <c r="B287" s="11" t="s">
+      <c r="B287" s="9" t="s">
         <v>1096</v>
       </c>
-      <c r="C287" s="13" t="s">
+      <c r="C287" s="11" t="s">
         <v>1097</v>
       </c>
-      <c r="D287" s="14" t="s">
+      <c r="D287" s="12" t="s">
         <v>1098</v>
       </c>
-      <c r="E287" s="13" t="s">
+      <c r="E287" s="11" t="s">
         <v>1099</v>
       </c>
-      <c r="F287" s="13" t="s">
+      <c r="F287" s="11" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="288" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A288" s="11">
+      <c r="A288" s="9">
         <v>200068</v>
       </c>
-      <c r="B288" s="11" t="s">
+      <c r="B288" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="C288" s="13" t="s">
+      <c r="C288" s="11" t="s">
         <v>1101</v>
       </c>
-      <c r="D288" s="13" t="s">
+      <c r="D288" s="11" t="s">
         <v>1102</v>
       </c>
-      <c r="E288" s="13" t="s">
+      <c r="E288" s="11" t="s">
         <v>1103</v>
       </c>
-      <c r="F288" s="13" t="s">
+      <c r="F288" s="11" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="289" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A289" s="11">
+      <c r="A289" s="9">
         <v>200069</v>
       </c>
-      <c r="B289" s="11" t="s">
+      <c r="B289" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="C289" s="14" t="s">
+      <c r="C289" s="12" t="s">
         <v>1083</v>
       </c>
-      <c r="D289" s="14" t="s">
+      <c r="D289" s="12" t="s">
         <v>1056</v>
       </c>
-      <c r="E289" s="13" t="s">
+      <c r="E289" s="11" t="s">
         <v>1057</v>
       </c>
-      <c r="F289" s="13" t="s">
+      <c r="F289" s="11" t="s">
         <v>1083</v>
       </c>
     </row>
     <row r="290" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A290" s="11">
+      <c r="A290" s="9">
         <v>200070</v>
       </c>
-      <c r="B290" s="11" t="s">
+      <c r="B290" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="C290" s="14" t="s">
+      <c r="C290" s="12" t="s">
         <v>1106</v>
       </c>
-      <c r="D290" s="14" t="s">
+      <c r="D290" s="12" t="s">
         <v>1107</v>
       </c>
-      <c r="E290" s="13" t="s">
+      <c r="E290" s="11" t="s">
         <v>1108</v>
       </c>
-      <c r="F290" s="13" t="s">
+      <c r="F290" s="11" t="s">
         <v>1106</v>
       </c>
     </row>
     <row r="291" s="2" customFormat="1" ht="18.75" customHeight="1" spans="1:6">
-      <c r="A291" s="11">
+      <c r="A291" s="9">
         <v>200071</v>
       </c>
-      <c r="B291" s="11" t="s">
+      <c r="B291" s="9" t="s">
         <v>1109</v>
       </c>
-      <c r="C291" s="14" t="s">
+      <c r="C291" s="12" t="s">
         <v>1110</v>
       </c>
-      <c r="D291" s="14" t="s">
+      <c r="D291" s="12" t="s">
         <v>1111</v>
       </c>
-      <c r="E291" s="13" t="s">
+      <c r="E291" s="11" t="s">
         <v>1112</v>
       </c>
-      <c r="F291" s="13" t="s">
+      <c r="F291" s="11" t="s">
         <v>1110</v>
       </c>
     </row>
@@ -11054,7 +11083,7 @@
       <c r="D302" s="3" t="s">
         <v>1152</v>
       </c>
-      <c r="E302" s="15" t="s">
+      <c r="E302" s="13" t="s">
         <v>1153</v>
       </c>
       <c r="F302" s="2" t="s">
@@ -11074,7 +11103,7 @@
       <c r="D303" s="3" t="s">
         <v>1156</v>
       </c>
-      <c r="E303" s="15" t="s">
+      <c r="E303" s="13" t="s">
         <v>1157</v>
       </c>
       <c r="F303" s="2" t="s">
@@ -11094,7 +11123,7 @@
       <c r="D304" s="3" t="s">
         <v>1160</v>
       </c>
-      <c r="E304" s="15" t="s">
+      <c r="E304" s="13" t="s">
         <v>1161</v>
       </c>
       <c r="F304" s="2" t="s">
@@ -11114,7 +11143,7 @@
       <c r="D305" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="E305" s="15" t="s">
+      <c r="E305" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="F305" s="2" t="s">
@@ -11134,7 +11163,7 @@
       <c r="D306" s="3" t="s">
         <v>1165</v>
       </c>
-      <c r="E306" s="15" t="s">
+      <c r="E306" s="13" t="s">
         <v>1166</v>
       </c>
       <c r="F306" s="2" t="s">
@@ -11154,7 +11183,7 @@
       <c r="D307" s="3" t="s">
         <v>1169</v>
       </c>
-      <c r="E307" s="15" t="s">
+      <c r="E307" s="13" t="s">
         <v>1170</v>
       </c>
       <c r="F307" s="2" t="s">
@@ -11174,7 +11203,7 @@
       <c r="D308" s="3" t="s">
         <v>1173</v>
       </c>
-      <c r="E308" s="15" t="s">
+      <c r="E308" s="13" t="s">
         <v>1174</v>
       </c>
       <c r="F308" s="2" t="s">
@@ -11194,7 +11223,7 @@
       <c r="D309" s="3" t="s">
         <v>1177</v>
       </c>
-      <c r="E309" s="15" t="s">
+      <c r="E309" s="13" t="s">
         <v>1178</v>
       </c>
       <c r="F309" s="2" t="s">
@@ -11214,7 +11243,7 @@
       <c r="D310" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="E310" s="15" t="s">
+      <c r="E310" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="F310" s="2" t="s">
@@ -11234,7 +11263,7 @@
       <c r="D311" s="3" t="s">
         <v>1182</v>
       </c>
-      <c r="E311" s="15" t="s">
+      <c r="E311" s="13" t="s">
         <v>1183</v>
       </c>
       <c r="F311" s="2" t="s">
@@ -11254,7 +11283,7 @@
       <c r="D312" s="3" t="s">
         <v>1186</v>
       </c>
-      <c r="E312" s="15" t="s">
+      <c r="E312" s="13" t="s">
         <v>1187</v>
       </c>
       <c r="F312" s="2" t="s">
@@ -11274,7 +11303,7 @@
       <c r="D313" s="3" t="s">
         <v>1190</v>
       </c>
-      <c r="E313" s="15" t="s">
+      <c r="E313" s="13" t="s">
         <v>1191</v>
       </c>
       <c r="F313" s="2" t="s">
@@ -11294,7 +11323,7 @@
       <c r="D314" s="3" t="s">
         <v>1194</v>
       </c>
-      <c r="E314" s="15" t="s">
+      <c r="E314" s="13" t="s">
         <v>1195</v>
       </c>
       <c r="F314" s="2" t="s">
@@ -11314,7 +11343,7 @@
       <c r="D315" s="3" t="s">
         <v>1198</v>
       </c>
-      <c r="E315" s="15" t="s">
+      <c r="E315" s="13" t="s">
         <v>1199</v>
       </c>
       <c r="F315" s="2" t="s">
@@ -11334,7 +11363,7 @@
       <c r="D316" s="3" t="s">
         <v>1202</v>
       </c>
-      <c r="E316" s="15" t="s">
+      <c r="E316" s="13" t="s">
         <v>1203</v>
       </c>
       <c r="F316" s="2" t="s">
@@ -11354,7 +11383,7 @@
       <c r="D317" s="3" t="s">
         <v>1206</v>
       </c>
-      <c r="E317" s="15" t="s">
+      <c r="E317" s="13" t="s">
         <v>1207</v>
       </c>
       <c r="F317" s="2" t="s">
@@ -11374,7 +11403,7 @@
       <c r="D318" s="3" t="s">
         <v>1210</v>
       </c>
-      <c r="E318" s="15" t="s">
+      <c r="E318" s="13" t="s">
         <v>1211</v>
       </c>
       <c r="F318" s="2" t="s">
@@ -11394,7 +11423,7 @@
       <c r="D319" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="E319" s="15" t="s">
+      <c r="E319" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="F319" s="2" t="s">
@@ -11414,7 +11443,7 @@
       <c r="D320" s="3" t="s">
         <v>1215</v>
       </c>
-      <c r="E320" s="15" t="s">
+      <c r="E320" s="13" t="s">
         <v>1216</v>
       </c>
       <c r="F320" s="2" t="s">
@@ -11434,7 +11463,7 @@
       <c r="D321" s="3" t="s">
         <v>1219</v>
       </c>
-      <c r="E321" s="15" t="s">
+      <c r="E321" s="13" t="s">
         <v>1220</v>
       </c>
       <c r="F321" s="2" t="s">
@@ -11454,7 +11483,7 @@
       <c r="D322" s="3" t="s">
         <v>1223</v>
       </c>
-      <c r="E322" s="15" t="s">
+      <c r="E322" s="13" t="s">
         <v>1224</v>
       </c>
       <c r="F322" s="2" t="s">
@@ -11474,7 +11503,7 @@
       <c r="D323" s="3" t="s">
         <v>1227</v>
       </c>
-      <c r="E323" s="15" t="s">
+      <c r="E323" s="13" t="s">
         <v>1228</v>
       </c>
       <c r="F323" s="2" t="s">
@@ -11494,7 +11523,7 @@
       <c r="D324" s="3" t="s">
         <v>1231</v>
       </c>
-      <c r="E324" s="15" t="s">
+      <c r="E324" s="13" t="s">
         <v>1232</v>
       </c>
       <c r="F324" s="2" t="s">
@@ -11514,7 +11543,7 @@
       <c r="D325" s="3" t="s">
         <v>1235</v>
       </c>
-      <c r="E325" s="15" t="s">
+      <c r="E325" s="13" t="s">
         <v>1236</v>
       </c>
       <c r="F325" s="2" t="s">
@@ -11534,7 +11563,7 @@
       <c r="D326" s="3" t="s">
         <v>1239</v>
       </c>
-      <c r="E326" s="15" t="s">
+      <c r="E326" s="13" t="s">
         <v>1240</v>
       </c>
       <c r="F326" s="2" t="s">
@@ -11554,7 +11583,7 @@
       <c r="D327" s="3" t="s">
         <v>1243</v>
       </c>
-      <c r="E327" s="15" t="s">
+      <c r="E327" s="13" t="s">
         <v>1244</v>
       </c>
       <c r="F327" s="2" t="s">
@@ -11574,7 +11603,7 @@
       <c r="D328" s="3" t="s">
         <v>1247</v>
       </c>
-      <c r="E328" s="15" t="s">
+      <c r="E328" s="13" t="s">
         <v>1247</v>
       </c>
       <c r="F328" s="2" t="s">
@@ -11594,7 +11623,7 @@
       <c r="D329" s="3" t="s">
         <v>1250</v>
       </c>
-      <c r="E329" s="15" t="s">
+      <c r="E329" s="13" t="s">
         <v>1251</v>
       </c>
       <c r="F329" s="2" t="s">
@@ -11614,7 +11643,7 @@
       <c r="D330" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="E330" s="15" t="s">
+      <c r="E330" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="F330" s="2" t="s">
@@ -11634,7 +11663,7 @@
       <c r="D331" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="E331" s="15" t="s">
+      <c r="E331" s="13" t="s">
         <v>1256</v>
       </c>
       <c r="F331" s="2" t="s">
@@ -11654,7 +11683,7 @@
       <c r="D332" s="3" t="s">
         <v>1259</v>
       </c>
-      <c r="E332" s="15" t="s">
+      <c r="E332" s="13" t="s">
         <v>1260</v>
       </c>
       <c r="F332" s="2" t="s">
@@ -11674,7 +11703,7 @@
       <c r="D333" s="3" t="s">
         <v>1263</v>
       </c>
-      <c r="E333" s="15" t="s">
+      <c r="E333" s="13" t="s">
         <v>1264</v>
       </c>
       <c r="F333" s="2" t="s">
@@ -11694,7 +11723,7 @@
       <c r="D334" s="3" t="s">
         <v>1267</v>
       </c>
-      <c r="E334" s="15" t="s">
+      <c r="E334" s="13" t="s">
         <v>1268</v>
       </c>
       <c r="F334" s="2" t="s">
@@ -11714,7 +11743,7 @@
       <c r="D335" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="E335" s="15" t="s">
+      <c r="E335" s="13" t="s">
         <v>1128</v>
       </c>
       <c r="F335" s="2" t="s">
@@ -11734,7 +11763,7 @@
       <c r="D336" s="3" t="s">
         <v>1272</v>
       </c>
-      <c r="E336" s="15" t="s">
+      <c r="E336" s="13" t="s">
         <v>1273</v>
       </c>
       <c r="F336" s="2" t="s">
@@ -11754,7 +11783,7 @@
       <c r="D337" s="3" t="s">
         <v>1276</v>
       </c>
-      <c r="E337" s="15" t="s">
+      <c r="E337" s="13" t="s">
         <v>1277</v>
       </c>
       <c r="F337" s="3" t="s">
@@ -11774,7 +11803,7 @@
       <c r="D338" s="3" t="s">
         <v>1280</v>
       </c>
-      <c r="E338" s="15" t="s">
+      <c r="E338" s="13" t="s">
         <v>1281</v>
       </c>
       <c r="F338" s="3" t="s">
@@ -11794,7 +11823,7 @@
       <c r="D339" s="3" t="s">
         <v>1284</v>
       </c>
-      <c r="E339" s="15" t="s">
+      <c r="E339" s="13" t="s">
         <v>1285</v>
       </c>
       <c r="F339" s="3" t="s">
@@ -11809,16 +11838,16 @@
       <c r="B341" s="3" t="s">
         <v>1286</v>
       </c>
-      <c r="C341" s="16" t="s">
+      <c r="C341" s="14" t="s">
         <v>1287</v>
       </c>
       <c r="D341" s="3" t="s">
         <v>1288</v>
       </c>
-      <c r="E341" s="16" t="s">
+      <c r="E341" s="14" t="s">
         <v>1287</v>
       </c>
-      <c r="F341" s="16" t="s">
+      <c r="F341" s="14" t="s">
         <v>1287</v>
       </c>
     </row>
@@ -11829,16 +11858,16 @@
       <c r="B342" s="3" t="s">
         <v>1289</v>
       </c>
-      <c r="C342" s="16" t="s">
+      <c r="C342" s="14" t="s">
         <v>1290</v>
       </c>
       <c r="D342" s="3" t="s">
         <v>1291</v>
       </c>
-      <c r="E342" s="16" t="s">
+      <c r="E342" s="14" t="s">
         <v>1290</v>
       </c>
-      <c r="F342" s="16" t="s">
+      <c r="F342" s="14" t="s">
         <v>1290</v>
       </c>
     </row>
@@ -12156,7 +12185,7 @@
       <c r="C363" s="2" t="s">
         <v>1351</v>
       </c>
-      <c r="D363" s="17" t="s">
+      <c r="D363" s="15" t="s">
         <v>1352</v>
       </c>
     </row>
@@ -12174,11 +12203,106 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="365" s="2" customFormat="1"/>
-    <row r="366" s="2" customFormat="1"/>
-    <row r="367" s="2" customFormat="1"/>
-    <row r="368" s="2" customFormat="1"/>
-    <row r="369" s="2" customFormat="1"/>
+    <row r="365" s="2" customFormat="1" spans="1:6">
+      <c r="A365" s="2">
+        <v>300024</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C365" s="16" t="s">
+        <v>1357</v>
+      </c>
+      <c r="D365" s="16" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E365" s="16" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F365" s="16" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="366" s="2" customFormat="1" spans="1:6">
+      <c r="A366" s="2">
+        <v>300025</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C366" s="16" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D366" s="16" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E366" s="16" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F366" s="16" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="367" s="2" customFormat="1" spans="1:6">
+      <c r="A367" s="2">
+        <v>300026</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C367" s="16" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D367" s="16" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E367" s="16" t="s">
+        <v>1361</v>
+      </c>
+      <c r="F367" s="16" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="368" s="2" customFormat="1" spans="1:6">
+      <c r="A368" s="2">
+        <v>300027</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C368" s="16" t="s">
+        <v>1363</v>
+      </c>
+      <c r="D368" s="16" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E368" s="16" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F368" s="16" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="369" s="2" customFormat="1" spans="1:6">
+      <c r="A369" s="2">
+        <v>300028</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C369" s="17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D369" s="17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E369" s="17" t="s">
+        <v>1365</v>
+      </c>
+      <c r="F369" s="17" t="s">
+        <v>1365</v>
+      </c>
+    </row>
     <row r="370" s="2" customFormat="1"/>
     <row r="371" s="2" customFormat="1"/>
     <row r="372" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat：udpate new tipsplaylist excel
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="1378">
   <si>
     <t>int</t>
   </si>
@@ -4140,6 +4140,42 @@
   </si>
   <si>
     <t>冰层</t>
+  </si>
+  <si>
+    <t>Tiptext001</t>
+  </si>
+  <si>
+    <t>全局提示一号机</t>
+  </si>
+  <si>
+    <t>Tiptext002</t>
+  </si>
+  <si>
+    <t>全局提示二号机</t>
+  </si>
+  <si>
+    <t>Tiptext003</t>
+  </si>
+  <si>
+    <t>全局提示三号机</t>
+  </si>
+  <si>
+    <t>Tiptext004</t>
+  </si>
+  <si>
+    <t>全局提示四号机</t>
+  </si>
+  <si>
+    <t>Tiptext005</t>
+  </si>
+  <si>
+    <t>全局提示五号机</t>
+  </si>
+  <si>
+    <t>Tiptext006</t>
+  </si>
+  <si>
+    <t>全局提示六号机</t>
   </si>
 </sst>
 </file>
@@ -5232,8 +5268,8 @@
   <sheetPr/>
   <dimension ref="A1:H676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D336" workbookViewId="0">
-      <selection activeCell="E359" sqref="E359"/>
+    <sheetView tabSelected="1" topLeftCell="A348" workbookViewId="0">
+      <selection activeCell="C381" sqref="C381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -12303,12 +12339,126 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="370" s="2" customFormat="1"/>
-    <row r="371" s="2" customFormat="1"/>
-    <row r="372" s="2" customFormat="1"/>
-    <row r="373" s="2" customFormat="1"/>
-    <row r="374" s="2" customFormat="1"/>
-    <row r="375" s="2" customFormat="1"/>
+    <row r="370" s="2" customFormat="1" spans="1:6">
+      <c r="A370" s="2">
+        <v>300029</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C370" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="D370" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E370" s="2" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F370" s="2" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="371" s="2" customFormat="1" spans="1:6">
+      <c r="A371" s="2">
+        <v>300030</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="D371" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E371" s="2" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F371" s="2" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="372" s="2" customFormat="1" spans="1:6">
+      <c r="A372" s="2">
+        <v>300031</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>1371</v>
+      </c>
+      <c r="D372" s="2" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E372" s="2" t="s">
+        <v>1371</v>
+      </c>
+      <c r="F372" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="373" s="2" customFormat="1" spans="1:6">
+      <c r="A373" s="2">
+        <v>300032</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C373" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D373" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="E373" s="2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F373" s="2" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="374" s="2" customFormat="1" spans="1:6">
+      <c r="A374" s="2">
+        <v>300033</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="D374" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="E374" s="2" t="s">
+        <v>1375</v>
+      </c>
+      <c r="F374" s="2" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="375" s="2" customFormat="1" spans="1:6">
+      <c r="A375" s="2">
+        <v>300034</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D375" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="E375" s="2" t="s">
+        <v>1377</v>
+      </c>
+      <c r="F375" s="2" t="s">
+        <v>1377</v>
+      </c>
+    </row>
     <row r="376" s="2" customFormat="1"/>
     <row r="377" s="2" customFormat="1"/>
     <row r="378" s="2" customFormat="1"/>

</xml_diff>

<commit_message>
feat：update language excel change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -4152,7 +4152,7 @@
     <t xml:space="preserve">Enable</t>
   </si>
   <si>
-    <t xml:space="preserve">啟動</t>
+    <t xml:space="preserve">启动</t>
   </si>
   <si>
     <t xml:space="preserve">Main_Scene_Name</t>
@@ -4935,8 +4935,8 @@
   </sheetPr>
   <dimension ref="A1:H676"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A408" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H418" activeCellId="0" sqref="H418"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A363" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D380" activeCellId="0" sqref="D380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat: update onlineshop ui
增加dv商店刷新按钮
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/Language_多语言表.xlsx
+++ b/dragon-verse/Excels/Language_多语言表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\v0.38.0.0.20240805170156\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\dragon-verse\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Editor\editor_v0.40.0.2.20241015185135\MetaWorldSaved\Saved\MetaWorld\Project\Edit\dragon-verse\dragon-verse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A57E44-22E6-42AB-8FD0-9E74D85AA78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECFDB97-4892-4A39-8DB0-5C04F9471E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2420" uniqueCount="1726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1729">
   <si>
     <t>int</t>
   </si>
@@ -4664,9 +4664,6 @@
     <t>取消（Esc）</t>
   </si>
   <si>
-    <t>Online_shop014</t>
-  </si>
-  <si>
     <t>Confirming</t>
   </si>
   <si>
@@ -5222,6 +5219,22 @@
   </si>
   <si>
     <t>龙域保卫战</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Online_shop014</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Online_shop015</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Refresh</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>刷新</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -5622,8 +5635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H676"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A487" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D501" sqref="D501"/>
+    <sheetView tabSelected="1" topLeftCell="A497" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D509" sqref="D509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -14183,19 +14196,19 @@
         <v>300095</v>
       </c>
       <c r="B436" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="C436" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="C436" s="2" t="s">
+      <c r="D436" s="2" t="s">
         <v>1541</v>
       </c>
-      <c r="D436" s="2" t="s">
-        <v>1542</v>
-      </c>
       <c r="E436" s="2" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="F436" s="2" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="437" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14203,19 +14216,19 @@
         <v>300096</v>
       </c>
       <c r="B437" s="4" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C437" s="22" t="s">
         <v>1543</v>
       </c>
-      <c r="C437" s="22" t="s">
+      <c r="D437" s="22" t="s">
         <v>1544</v>
       </c>
-      <c r="D437" s="22" t="s">
-        <v>1545</v>
-      </c>
       <c r="E437" s="22" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="F437" s="22" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="438" spans="1:7" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14223,19 +14236,19 @@
         <v>300097</v>
       </c>
       <c r="B438" s="4" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C438" s="22" t="s">
         <v>1546</v>
       </c>
-      <c r="C438" s="22" t="s">
+      <c r="D438" s="22" t="s">
         <v>1547</v>
       </c>
-      <c r="D438" s="22" t="s">
-        <v>1548</v>
-      </c>
       <c r="E438" s="22" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="F438" s="22" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="439" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14243,19 +14256,19 @@
         <v>300098</v>
       </c>
       <c r="B439" s="4" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C439" s="22" t="s">
         <v>1549</v>
       </c>
-      <c r="C439" s="22" t="s">
+      <c r="D439" s="22" t="s">
         <v>1550</v>
       </c>
-      <c r="D439" s="22" t="s">
-        <v>1551</v>
-      </c>
       <c r="E439" s="22" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="F439" s="22" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="440" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14263,19 +14276,19 @@
         <v>300099</v>
       </c>
       <c r="B440" s="4" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C440" s="22" t="s">
         <v>1552</v>
       </c>
-      <c r="C440" s="22" t="s">
+      <c r="D440" s="22" t="s">
         <v>1553</v>
       </c>
-      <c r="D440" s="22" t="s">
-        <v>1554</v>
-      </c>
       <c r="E440" s="22" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="F440" s="22" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="441" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14283,19 +14296,19 @@
         <v>300100</v>
       </c>
       <c r="B441" s="4" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C441" s="22" t="s">
         <v>1555</v>
       </c>
-      <c r="C441" s="22" t="s">
+      <c r="D441" s="22" t="s">
         <v>1556</v>
       </c>
-      <c r="D441" s="22" t="s">
-        <v>1557</v>
-      </c>
       <c r="E441" s="22" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="F441" s="22" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="442" spans="1:7" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14303,19 +14316,19 @@
         <v>300101</v>
       </c>
       <c r="B442" s="4" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C442" s="22" t="s">
         <v>1558</v>
       </c>
-      <c r="C442" s="22" t="s">
+      <c r="D442" s="22" t="s">
         <v>1559</v>
       </c>
-      <c r="D442" s="22" t="s">
-        <v>1560</v>
-      </c>
       <c r="E442" s="22" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="F442" s="22" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="443" spans="1:7" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14323,19 +14336,19 @@
         <v>300102</v>
       </c>
       <c r="B443" s="4" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C443" s="22" t="s">
         <v>1561</v>
       </c>
-      <c r="C443" s="22" t="s">
+      <c r="D443" s="22" t="s">
         <v>1562</v>
       </c>
-      <c r="D443" s="22" t="s">
-        <v>1563</v>
-      </c>
       <c r="E443" s="22" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="F443" s="22" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="444" spans="1:7" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14343,19 +14356,19 @@
         <v>300103</v>
       </c>
       <c r="B444" s="4" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C444" s="22" t="s">
         <v>1564</v>
       </c>
-      <c r="C444" s="22" t="s">
+      <c r="D444" s="22" t="s">
         <v>1565</v>
       </c>
-      <c r="D444" s="22" t="s">
-        <v>1566</v>
-      </c>
       <c r="E444" s="22" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="F444" s="22" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="445" spans="1:7" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14363,19 +14376,19 @@
         <v>300104</v>
       </c>
       <c r="B445" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C445" s="22" t="s">
         <v>1567</v>
       </c>
-      <c r="C445" s="22" t="s">
+      <c r="D445" s="22" t="s">
         <v>1568</v>
       </c>
-      <c r="D445" s="22" t="s">
-        <v>1569</v>
-      </c>
       <c r="E445" s="22" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="F445" s="22" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="446" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14383,19 +14396,19 @@
         <v>300105</v>
       </c>
       <c r="B446" s="4" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C446" s="22" t="s">
         <v>1570</v>
       </c>
-      <c r="C446" s="22" t="s">
+      <c r="D446" s="22" t="s">
         <v>1571</v>
       </c>
-      <c r="D446" s="22" t="s">
-        <v>1572</v>
-      </c>
       <c r="E446" s="22" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="F446" s="22" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="447" spans="1:7" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14403,19 +14416,19 @@
         <v>300106</v>
       </c>
       <c r="B447" s="4" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C447" s="22" t="s">
         <v>1573</v>
       </c>
-      <c r="C447" s="22" t="s">
+      <c r="D447" s="22" t="s">
         <v>1574</v>
       </c>
-      <c r="D447" s="22" t="s">
-        <v>1575</v>
-      </c>
       <c r="E447" s="22" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F447" s="22" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="448" spans="1:7" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14423,19 +14436,19 @@
         <v>300107</v>
       </c>
       <c r="B448" s="4" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C448" s="22" t="s">
         <v>1576</v>
       </c>
-      <c r="C448" s="22" t="s">
+      <c r="D448" s="22" t="s">
         <v>1577</v>
       </c>
-      <c r="D448" s="22" t="s">
-        <v>1578</v>
-      </c>
       <c r="E448" s="22" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="F448" s="22" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="449" spans="1:6" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14443,19 +14456,19 @@
         <v>300108</v>
       </c>
       <c r="B449" s="4" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C449" s="22" t="s">
         <v>1579</v>
       </c>
-      <c r="C449" s="22" t="s">
+      <c r="D449" s="22" t="s">
         <v>1580</v>
       </c>
-      <c r="D449" s="22" t="s">
-        <v>1581</v>
-      </c>
       <c r="E449" s="22" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="F449" s="22" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="450" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14463,19 +14476,19 @@
         <v>300109</v>
       </c>
       <c r="B450" s="4" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C450" s="22" t="s">
         <v>1582</v>
       </c>
-      <c r="C450" s="22" t="s">
+      <c r="D450" s="22" t="s">
         <v>1583</v>
       </c>
-      <c r="D450" s="22" t="s">
-        <v>1584</v>
-      </c>
       <c r="E450" s="22" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="F450" s="22" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="451" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14483,19 +14496,19 @@
         <v>300110</v>
       </c>
       <c r="B451" s="4" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C451" s="22" t="s">
         <v>1585</v>
       </c>
-      <c r="C451" s="22" t="s">
+      <c r="D451" s="22" t="s">
         <v>1586</v>
       </c>
-      <c r="D451" s="22" t="s">
-        <v>1587</v>
-      </c>
       <c r="E451" s="22" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="F451" s="22" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="452" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14503,19 +14516,19 @@
         <v>300111</v>
       </c>
       <c r="B452" s="4" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C452" s="22" t="s">
         <v>1588</v>
       </c>
-      <c r="C452" s="22" t="s">
+      <c r="D452" s="22" t="s">
         <v>1589</v>
       </c>
-      <c r="D452" s="22" t="s">
-        <v>1590</v>
-      </c>
       <c r="E452" s="22" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="F452" s="22" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="453" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14523,19 +14536,19 @@
         <v>300112</v>
       </c>
       <c r="B453" s="4" t="s">
+        <v>1590</v>
+      </c>
+      <c r="C453" s="22" t="s">
         <v>1591</v>
       </c>
-      <c r="C453" s="22" t="s">
+      <c r="D453" s="22" t="s">
         <v>1592</v>
       </c>
-      <c r="D453" s="22" t="s">
-        <v>1593</v>
-      </c>
       <c r="E453" s="22" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="F453" s="22" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="454" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14543,19 +14556,19 @@
         <v>300113</v>
       </c>
       <c r="B454" s="4" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C454" s="22" t="s">
         <v>1594</v>
       </c>
-      <c r="C454" s="22" t="s">
+      <c r="D454" s="22" t="s">
         <v>1595</v>
       </c>
-      <c r="D454" s="22" t="s">
-        <v>1596</v>
-      </c>
       <c r="E454" s="22" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="F454" s="22" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="455" spans="1:6" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14563,19 +14576,19 @@
         <v>300114</v>
       </c>
       <c r="B455" s="4" t="s">
+        <v>1596</v>
+      </c>
+      <c r="C455" s="22" t="s">
         <v>1597</v>
       </c>
-      <c r="C455" s="22" t="s">
+      <c r="D455" s="22" t="s">
         <v>1598</v>
       </c>
-      <c r="D455" s="22" t="s">
-        <v>1599</v>
-      </c>
       <c r="E455" s="22" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="F455" s="22" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="456" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14583,19 +14596,19 @@
         <v>300115</v>
       </c>
       <c r="B456" s="4" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C456" s="22" t="s">
         <v>1600</v>
       </c>
-      <c r="C456" s="22" t="s">
+      <c r="D456" s="22" t="s">
         <v>1601</v>
       </c>
-      <c r="D456" s="22" t="s">
-        <v>1602</v>
-      </c>
       <c r="E456" s="22" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="F456" s="22" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="457" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14603,19 +14616,19 @@
         <v>300116</v>
       </c>
       <c r="B457" s="4" t="s">
+        <v>1602</v>
+      </c>
+      <c r="C457" s="22" t="s">
         <v>1603</v>
       </c>
-      <c r="C457" s="22" t="s">
+      <c r="D457" s="22" t="s">
         <v>1604</v>
       </c>
-      <c r="D457" s="22" t="s">
-        <v>1605</v>
-      </c>
       <c r="E457" s="22" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="F457" s="22" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="458" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14623,19 +14636,19 @@
         <v>300117</v>
       </c>
       <c r="B458" s="4" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C458" s="22" t="s">
         <v>1606</v>
       </c>
-      <c r="C458" s="22" t="s">
+      <c r="D458" s="22" t="s">
         <v>1607</v>
       </c>
-      <c r="D458" s="22" t="s">
-        <v>1608</v>
-      </c>
       <c r="E458" s="22" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="F458" s="22" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="459" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14643,7 +14656,7 @@
         <v>300118</v>
       </c>
       <c r="B459" s="4" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="460" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14651,7 +14664,7 @@
         <v>300119</v>
       </c>
       <c r="B460" s="4" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="461" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14659,7 +14672,7 @@
         <v>300120</v>
       </c>
       <c r="B461" s="4" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="462" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14667,19 +14680,19 @@
         <v>300121</v>
       </c>
       <c r="B462" s="4" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C462" s="22" t="s">
         <v>1612</v>
       </c>
-      <c r="C462" s="22" t="s">
+      <c r="D462" s="22" t="s">
         <v>1613</v>
       </c>
-      <c r="D462" s="22" t="s">
-        <v>1614</v>
-      </c>
       <c r="E462" s="22" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="F462" s="22" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="463" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14687,19 +14700,19 @@
         <v>300122</v>
       </c>
       <c r="B463" s="4" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C463" s="22" t="s">
         <v>1615</v>
       </c>
-      <c r="C463" s="22" t="s">
+      <c r="D463" s="22" t="s">
         <v>1616</v>
       </c>
-      <c r="D463" s="22" t="s">
-        <v>1617</v>
-      </c>
       <c r="E463" s="22" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="F463" s="22" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="464" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14707,7 +14720,7 @@
         <v>300123</v>
       </c>
       <c r="B464" s="4" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="465" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14715,7 +14728,7 @@
         <v>300124</v>
       </c>
       <c r="B465" s="4" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="466" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14723,7 +14736,7 @@
         <v>300125</v>
       </c>
       <c r="B466" s="4" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="467" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14731,19 +14744,19 @@
         <v>300126</v>
       </c>
       <c r="B467" s="4" t="s">
+        <v>1620</v>
+      </c>
+      <c r="C467" s="22" t="s">
         <v>1621</v>
       </c>
-      <c r="C467" s="22" t="s">
+      <c r="D467" s="22" t="s">
         <v>1622</v>
       </c>
-      <c r="D467" s="22" t="s">
-        <v>1623</v>
-      </c>
       <c r="E467" s="22" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="F467" s="22" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="468" spans="1:6" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14751,19 +14764,19 @@
         <v>300127</v>
       </c>
       <c r="B468" s="4" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C468" s="22" t="s">
         <v>1624</v>
       </c>
-      <c r="C468" s="22" t="s">
+      <c r="D468" s="22" t="s">
         <v>1625</v>
       </c>
-      <c r="D468" s="22" t="s">
-        <v>1626</v>
-      </c>
       <c r="E468" s="22" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="F468" s="22" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="469" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14771,7 +14784,7 @@
         <v>300128</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="470" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14779,7 +14792,7 @@
         <v>300129</v>
       </c>
       <c r="B470" s="4" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="471" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14787,7 +14800,7 @@
         <v>300130</v>
       </c>
       <c r="B471" s="4" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="472" spans="1:6" s="2" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
@@ -14795,19 +14808,19 @@
         <v>300131</v>
       </c>
       <c r="B472" s="4" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C472" s="22" t="s">
         <v>1630</v>
       </c>
-      <c r="C472" s="22" t="s">
+      <c r="D472" s="22" t="s">
         <v>1631</v>
       </c>
-      <c r="D472" s="22" t="s">
-        <v>1632</v>
-      </c>
       <c r="E472" s="22" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="F472" s="22" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="473" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14815,19 +14828,19 @@
         <v>300132</v>
       </c>
       <c r="B473" s="4" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C473" s="22" t="s">
         <v>1633</v>
       </c>
-      <c r="C473" s="22" t="s">
+      <c r="D473" s="22" t="s">
         <v>1634</v>
       </c>
-      <c r="D473" s="22" t="s">
-        <v>1635</v>
-      </c>
       <c r="E473" s="22" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="F473" s="22" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="474" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14835,7 +14848,7 @@
         <v>300133</v>
       </c>
       <c r="B474" s="4" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="475" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14843,7 +14856,7 @@
         <v>300134</v>
       </c>
       <c r="B475" s="4" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="476" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -14851,7 +14864,7 @@
         <v>300135</v>
       </c>
       <c r="B476" s="4" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="477" spans="1:6" s="2" customFormat="1" ht="115.5" x14ac:dyDescent="0.35">
@@ -14859,19 +14872,19 @@
         <v>300136</v>
       </c>
       <c r="B477" s="4" t="s">
+        <v>1638</v>
+      </c>
+      <c r="C477" s="22" t="s">
         <v>1639</v>
       </c>
-      <c r="C477" s="22" t="s">
+      <c r="D477" s="22" t="s">
         <v>1640</v>
       </c>
-      <c r="D477" s="22" t="s">
-        <v>1641</v>
-      </c>
       <c r="E477" s="22" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="F477" s="22" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="478" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14879,19 +14892,19 @@
         <v>300137</v>
       </c>
       <c r="B478" s="4" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C478" s="22" t="s">
         <v>1642</v>
       </c>
-      <c r="C478" s="22" t="s">
+      <c r="D478" s="21" t="s">
         <v>1643</v>
       </c>
-      <c r="D478" s="21" t="s">
-        <v>1644</v>
-      </c>
       <c r="E478" s="22" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="F478" s="22" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="479" spans="1:6" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.35">
@@ -14899,19 +14912,19 @@
         <v>300138</v>
       </c>
       <c r="B479" s="4" t="s">
+        <v>1644</v>
+      </c>
+      <c r="C479" s="22" t="s">
         <v>1645</v>
       </c>
-      <c r="C479" s="22" t="s">
+      <c r="D479" s="22" t="s">
         <v>1646</v>
       </c>
-      <c r="D479" s="22" t="s">
-        <v>1647</v>
-      </c>
       <c r="E479" s="22" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="F479" s="22" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="480" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14919,19 +14932,19 @@
         <v>300139</v>
       </c>
       <c r="B480" s="4" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C480" s="22" t="s">
         <v>1648</v>
       </c>
-      <c r="C480" s="22" t="s">
+      <c r="D480" s="22" t="s">
         <v>1649</v>
       </c>
-      <c r="D480" s="22" t="s">
-        <v>1650</v>
-      </c>
       <c r="E480" s="22" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="F480" s="22" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="481" spans="1:6" s="2" customFormat="1" ht="99" x14ac:dyDescent="0.35">
@@ -14939,19 +14952,19 @@
         <v>300140</v>
       </c>
       <c r="B481" s="4" t="s">
+        <v>1650</v>
+      </c>
+      <c r="C481" s="22" t="s">
         <v>1651</v>
       </c>
-      <c r="C481" s="22" t="s">
+      <c r="D481" s="22" t="s">
         <v>1652</v>
       </c>
-      <c r="D481" s="22" t="s">
-        <v>1653</v>
-      </c>
       <c r="E481" s="22" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="F481" s="22" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="482" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -14959,19 +14972,19 @@
         <v>300141</v>
       </c>
       <c r="B482" s="4" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C482" s="22" t="s">
         <v>1654</v>
       </c>
-      <c r="C482" s="22" t="s">
+      <c r="D482" s="22" t="s">
         <v>1655</v>
       </c>
-      <c r="D482" s="22" t="s">
-        <v>1656</v>
-      </c>
       <c r="E482" s="22" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="F482" s="22" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="483" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14979,19 +14992,19 @@
         <v>300142</v>
       </c>
       <c r="B483" s="4" t="s">
+        <v>1656</v>
+      </c>
+      <c r="C483" s="22" t="s">
         <v>1657</v>
       </c>
-      <c r="C483" s="22" t="s">
+      <c r="D483" s="22" t="s">
         <v>1658</v>
       </c>
-      <c r="D483" s="22" t="s">
-        <v>1659</v>
-      </c>
       <c r="E483" s="22" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="F483" s="22" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="484" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -14999,19 +15012,19 @@
         <v>300143</v>
       </c>
       <c r="B484" s="4" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C484" s="22" t="s">
         <v>1660</v>
       </c>
-      <c r="C484" s="22" t="s">
+      <c r="D484" s="22" t="s">
         <v>1661</v>
       </c>
-      <c r="D484" s="22" t="s">
-        <v>1662</v>
-      </c>
       <c r="E484" s="22" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="F484" s="22" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="485" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -15019,19 +15032,19 @@
         <v>300144</v>
       </c>
       <c r="B485" s="4" t="s">
+        <v>1662</v>
+      </c>
+      <c r="C485" s="22" t="s">
         <v>1663</v>
       </c>
-      <c r="C485" s="22" t="s">
+      <c r="D485" s="22" t="s">
         <v>1664</v>
       </c>
-      <c r="D485" s="22" t="s">
-        <v>1665</v>
-      </c>
       <c r="E485" s="22" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="F485" s="22" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="486" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -15039,19 +15052,19 @@
         <v>300145</v>
       </c>
       <c r="B486" s="4" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C486" s="22" t="s">
         <v>1666</v>
       </c>
-      <c r="C486" s="22" t="s">
+      <c r="D486" s="22" t="s">
         <v>1667</v>
       </c>
-      <c r="D486" s="22" t="s">
-        <v>1668</v>
-      </c>
       <c r="E486" s="22" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="F486" s="22" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="487" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -15059,19 +15072,19 @@
         <v>300146</v>
       </c>
       <c r="B487" s="4" t="s">
+        <v>1668</v>
+      </c>
+      <c r="C487" s="22" t="s">
         <v>1669</v>
       </c>
-      <c r="C487" s="22" t="s">
+      <c r="D487" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="D487" s="2" t="s">
-        <v>1671</v>
-      </c>
       <c r="E487" s="22" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="F487" s="22" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="488" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -15079,19 +15092,19 @@
         <v>300147</v>
       </c>
       <c r="B488" s="4" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C488" s="22" t="s">
         <v>1672</v>
       </c>
-      <c r="C488" s="22" t="s">
+      <c r="D488" s="22" t="s">
         <v>1673</v>
       </c>
-      <c r="D488" s="22" t="s">
-        <v>1674</v>
-      </c>
       <c r="E488" s="22" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="F488" s="22" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="489" spans="1:6" s="2" customFormat="1" ht="82.5" x14ac:dyDescent="0.35">
@@ -15099,19 +15112,19 @@
         <v>300148</v>
       </c>
       <c r="B489" s="4" t="s">
+        <v>1674</v>
+      </c>
+      <c r="C489" s="22" t="s">
         <v>1675</v>
       </c>
-      <c r="C489" s="22" t="s">
+      <c r="D489" s="22" t="s">
         <v>1676</v>
       </c>
-      <c r="D489" s="22" t="s">
-        <v>1677</v>
-      </c>
       <c r="E489" s="22" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="F489" s="22" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="490" spans="1:6" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.35">
@@ -15119,19 +15132,19 @@
         <v>300149</v>
       </c>
       <c r="B490" s="4" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C490" s="22" t="s">
         <v>1678</v>
       </c>
-      <c r="C490" s="22" t="s">
+      <c r="D490" s="22" t="s">
         <v>1679</v>
       </c>
-      <c r="D490" s="22" t="s">
-        <v>1680</v>
-      </c>
       <c r="E490" s="22" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="F490" s="22" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="491" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15139,19 +15152,19 @@
         <v>300150</v>
       </c>
       <c r="B491" s="18" t="s">
+        <v>1680</v>
+      </c>
+      <c r="C491" s="3" t="s">
         <v>1681</v>
       </c>
-      <c r="C491" s="3" t="s">
+      <c r="D491" s="2" t="s">
         <v>1682</v>
       </c>
-      <c r="D491" s="2" t="s">
-        <v>1683</v>
-      </c>
       <c r="E491" s="2" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="F491" s="2" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="492" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15159,19 +15172,19 @@
         <v>300151</v>
       </c>
       <c r="B492" s="18" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C492" s="3" t="s">
         <v>1684</v>
       </c>
-      <c r="C492" s="3" t="s">
+      <c r="D492" s="2" t="s">
         <v>1685</v>
       </c>
-      <c r="D492" s="2" t="s">
-        <v>1686</v>
-      </c>
       <c r="E492" s="2" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="F492" s="2" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="493" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15179,19 +15192,19 @@
         <v>300152</v>
       </c>
       <c r="B493" s="18" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C493" s="3" t="s">
         <v>1687</v>
       </c>
-      <c r="C493" s="3" t="s">
+      <c r="D493" s="3" t="s">
         <v>1688</v>
       </c>
-      <c r="D493" s="3" t="s">
-        <v>1689</v>
-      </c>
       <c r="E493" s="2" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="F493" s="2" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="494" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15199,19 +15212,19 @@
         <v>300153</v>
       </c>
       <c r="B494" s="18" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C494" s="3" t="s">
         <v>1690</v>
       </c>
-      <c r="C494" s="3" t="s">
+      <c r="D494" s="2" t="s">
         <v>1691</v>
       </c>
-      <c r="D494" s="2" t="s">
-        <v>1692</v>
-      </c>
       <c r="E494" s="2" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="F494" s="2" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="495" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15219,19 +15232,19 @@
         <v>300154</v>
       </c>
       <c r="B495" s="18" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C495" s="3" t="s">
         <v>1693</v>
       </c>
-      <c r="C495" s="3" t="s">
+      <c r="D495" s="2" t="s">
         <v>1694</v>
       </c>
-      <c r="D495" s="2" t="s">
-        <v>1695</v>
-      </c>
       <c r="E495" s="2" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="F495" s="2" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="496" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15239,19 +15252,19 @@
         <v>300155</v>
       </c>
       <c r="B496" s="18" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C496" s="3" t="s">
         <v>1696</v>
       </c>
-      <c r="C496" s="3" t="s">
+      <c r="D496" s="3" t="s">
         <v>1697</v>
       </c>
-      <c r="D496" s="3" t="s">
-        <v>1698</v>
-      </c>
       <c r="E496" s="2" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="F496" s="2" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="497" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15259,19 +15272,19 @@
         <v>300156</v>
       </c>
       <c r="B497" s="18" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C497" s="3" t="s">
         <v>1699</v>
       </c>
-      <c r="C497" s="3" t="s">
+      <c r="D497" s="2" t="s">
         <v>1700</v>
       </c>
-      <c r="D497" s="2" t="s">
-        <v>1701</v>
-      </c>
       <c r="E497" s="2" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="F497" s="2" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="498" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15279,19 +15292,19 @@
         <v>300157</v>
       </c>
       <c r="B498" s="18" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C498" s="3" t="s">
         <v>1702</v>
       </c>
-      <c r="C498" s="3" t="s">
+      <c r="D498" s="2" t="s">
         <v>1703</v>
       </c>
-      <c r="D498" s="2" t="s">
-        <v>1704</v>
-      </c>
       <c r="E498" s="2" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="F498" s="2" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="499" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15299,19 +15312,19 @@
         <v>300158</v>
       </c>
       <c r="B499" s="18" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C499" s="3" t="s">
         <v>1705</v>
       </c>
-      <c r="C499" s="3" t="s">
+      <c r="D499" s="2" t="s">
         <v>1706</v>
       </c>
-      <c r="D499" s="2" t="s">
-        <v>1707</v>
-      </c>
       <c r="E499" s="2" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="F499" s="2" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
     </row>
     <row r="500" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15319,19 +15332,19 @@
         <v>300159</v>
       </c>
       <c r="B500" s="18" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C500" s="3" t="s">
         <v>1708</v>
       </c>
-      <c r="C500" s="3" t="s">
+      <c r="D500" s="2" t="s">
         <v>1709</v>
       </c>
-      <c r="D500" s="2" t="s">
-        <v>1710</v>
-      </c>
       <c r="E500" s="2" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="F500" s="2" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="501" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15339,19 +15352,19 @@
         <v>300160</v>
       </c>
       <c r="B501" s="18" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C501" s="3" t="s">
         <v>1711</v>
       </c>
-      <c r="C501" s="3" t="s">
+      <c r="D501" s="2" t="s">
         <v>1712</v>
       </c>
-      <c r="D501" s="2" t="s">
-        <v>1713</v>
-      </c>
       <c r="E501" s="2" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="F501" s="2" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="502" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15359,19 +15372,19 @@
         <v>300161</v>
       </c>
       <c r="B502" s="18" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C502" s="3" t="s">
         <v>1714</v>
       </c>
-      <c r="C502" s="3" t="s">
+      <c r="D502" s="2" t="s">
         <v>1715</v>
       </c>
-      <c r="D502" s="2" t="s">
-        <v>1716</v>
-      </c>
       <c r="E502" s="2" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="F502" s="2" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="503" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15379,19 +15392,19 @@
         <v>300162</v>
       </c>
       <c r="B503" s="18" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C503" s="3" t="s">
         <v>1717</v>
       </c>
-      <c r="C503" s="3" t="s">
+      <c r="D503" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="D503" s="2" t="s">
-        <v>1719</v>
-      </c>
       <c r="E503" s="2" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="F503" s="2" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="504" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15399,19 +15412,19 @@
         <v>300163</v>
       </c>
       <c r="B504" s="18" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C504" s="3" t="s">
         <v>1720</v>
       </c>
-      <c r="C504" s="3" t="s">
+      <c r="D504" s="2" t="s">
         <v>1721</v>
       </c>
-      <c r="D504" s="2" t="s">
-        <v>1722</v>
-      </c>
       <c r="E504" s="2" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="F504" s="2" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="505" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -15419,22 +15432,41 @@
         <v>300164</v>
       </c>
       <c r="B505" s="29" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C505" s="3" t="s">
         <v>1723</v>
       </c>
-      <c r="C505" s="3" t="s">
+      <c r="D505" s="3" t="s">
         <v>1724</v>
       </c>
-      <c r="D505" s="3" t="s">
-        <v>1725</v>
-      </c>
       <c r="E505" s="3" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="F505" s="3" t="s">
-        <v>1725</v>
-      </c>
-    </row>
-    <row r="506" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A506" s="2">
+        <v>300165</v>
+      </c>
+      <c r="B506" s="3" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C506" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D506" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E506" s="3" t="s">
+        <v>1728</v>
+      </c>
+      <c r="F506" s="3" t="s">
+        <v>1728</v>
+      </c>
+    </row>
     <row r="507" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="508" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="509" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35"/>

</xml_diff>